<commit_message>
Updates example data for QA_Method_Writer
</commit_message>
<xml_diff>
--- a/QuantAnalysis/example_data_EIC_RT.xlsx
+++ b/QuantAnalysis/example_data_EIC_RT.xlsx
@@ -4,17 +4,18 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="45" windowWidth="20115" windowHeight="11310"/>
+    <workbookView xWindow="240" yWindow="45" windowWidth="20115" windowHeight="11310" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="5" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="6" r:id="rId2"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="12">
   <si>
     <t>1; 2</t>
   </si>
@@ -35,6 +36,21 @@
   </si>
   <si>
     <t>Precursor ions</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>PI</t>
+  </si>
+  <si>
+    <t>z</t>
+  </si>
+  <si>
+    <t>AVG_RT</t>
+  </si>
+  <si>
+    <t>AVG_RTW</t>
   </si>
 </sst>
 </file>
@@ -383,9 +399,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D143"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2147,4 +2161,2200 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E143"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I120" sqref="I120"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="16.5703125" customWidth="1"/>
+    <col min="3" max="3" width="8.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>94</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="1">
+        <v>19.8</v>
+      </c>
+      <c r="E2" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>95</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1">
+        <v>21.4</v>
+      </c>
+      <c r="E3" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>96</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="1">
+        <v>29.7</v>
+      </c>
+      <c r="E4" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>97</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="1">
+        <v>30.6</v>
+      </c>
+      <c r="E5" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>98</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="1">
+        <v>37.200000000000003</v>
+      </c>
+      <c r="E6" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>99</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" s="1">
+        <v>45.6</v>
+      </c>
+      <c r="E7" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8" s="2">
+        <v>1018.4</v>
+      </c>
+      <c r="C8">
+        <v>2</v>
+      </c>
+      <c r="D8" s="1">
+        <v>30.6</v>
+      </c>
+      <c r="E8" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>2</v>
+      </c>
+      <c r="B9" s="2">
+        <v>1022.4</v>
+      </c>
+      <c r="C9">
+        <v>2</v>
+      </c>
+      <c r="D9" s="1">
+        <v>20.5</v>
+      </c>
+      <c r="E9" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>3</v>
+      </c>
+      <c r="B10" s="2">
+        <v>1038.9000000000001</v>
+      </c>
+      <c r="C10">
+        <v>2</v>
+      </c>
+      <c r="D10" s="1">
+        <v>29</v>
+      </c>
+      <c r="E10" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>4</v>
+      </c>
+      <c r="B11" s="2">
+        <v>1038.9000000000001</v>
+      </c>
+      <c r="D11" s="1">
+        <v>32.1</v>
+      </c>
+      <c r="E11" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>5</v>
+      </c>
+      <c r="B12" s="2">
+        <v>1038.9000000000001</v>
+      </c>
+      <c r="D12" s="1">
+        <v>35</v>
+      </c>
+      <c r="E12" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>6</v>
+      </c>
+      <c r="B13" s="2">
+        <v>1038.9000000000001</v>
+      </c>
+      <c r="D13" s="1">
+        <v>36.5</v>
+      </c>
+      <c r="E13" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>7</v>
+      </c>
+      <c r="B14" s="2">
+        <v>1038.9000000000001</v>
+      </c>
+      <c r="D14" s="1">
+        <v>39.799999999999997</v>
+      </c>
+      <c r="E14" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>8</v>
+      </c>
+      <c r="B15" s="2">
+        <v>1046.9000000000001</v>
+      </c>
+      <c r="C15">
+        <v>2</v>
+      </c>
+      <c r="D15" s="1">
+        <v>17.5</v>
+      </c>
+      <c r="E15" s="1">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>9</v>
+      </c>
+      <c r="B16" s="2">
+        <v>1046.9000000000001</v>
+      </c>
+      <c r="D16" s="1">
+        <v>21.3</v>
+      </c>
+      <c r="E16" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>10</v>
+      </c>
+      <c r="B17" s="2">
+        <v>1046.9000000000001</v>
+      </c>
+      <c r="D17" s="1">
+        <v>29.9</v>
+      </c>
+      <c r="E17" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>11</v>
+      </c>
+      <c r="B18" s="2">
+        <v>1059.4000000000001</v>
+      </c>
+      <c r="C18">
+        <v>2</v>
+      </c>
+      <c r="D18" s="1">
+        <v>22.3</v>
+      </c>
+      <c r="E18" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>12</v>
+      </c>
+      <c r="B19" s="2">
+        <v>1067.4000000000001</v>
+      </c>
+      <c r="C19">
+        <v>2</v>
+      </c>
+      <c r="D19" s="1">
+        <v>19.899999999999999</v>
+      </c>
+      <c r="E19" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>13</v>
+      </c>
+      <c r="B20" s="2">
+        <v>1067.4000000000001</v>
+      </c>
+      <c r="D20" s="1">
+        <v>25.1</v>
+      </c>
+      <c r="E20" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>14</v>
+      </c>
+      <c r="B21" s="2">
+        <v>1083.9000000000001</v>
+      </c>
+      <c r="C21">
+        <v>2</v>
+      </c>
+      <c r="D21" s="1">
+        <v>20.399999999999999</v>
+      </c>
+      <c r="E21" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>15</v>
+      </c>
+      <c r="B22" s="2">
+        <v>1111.4000000000001</v>
+      </c>
+      <c r="C22">
+        <v>2</v>
+      </c>
+      <c r="D22" s="1">
+        <v>29.7</v>
+      </c>
+      <c r="E22" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>16</v>
+      </c>
+      <c r="B23" s="2">
+        <v>1111.4000000000001</v>
+      </c>
+      <c r="D23" s="1">
+        <v>37.700000000000003</v>
+      </c>
+      <c r="E23" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>17</v>
+      </c>
+      <c r="B24" s="2">
+        <v>1111.4000000000001</v>
+      </c>
+      <c r="D24" s="1">
+        <v>44.2</v>
+      </c>
+      <c r="E24" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>18</v>
+      </c>
+      <c r="B25" s="2">
+        <v>1119.9000000000001</v>
+      </c>
+      <c r="C25">
+        <v>2</v>
+      </c>
+      <c r="D25" s="1">
+        <v>21.6</v>
+      </c>
+      <c r="E25" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>19</v>
+      </c>
+      <c r="B26" s="2">
+        <v>1119.9000000000001</v>
+      </c>
+      <c r="D26" s="1">
+        <v>25.5</v>
+      </c>
+      <c r="E26" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>20</v>
+      </c>
+      <c r="B27" s="2">
+        <v>1119.9000000000001</v>
+      </c>
+      <c r="D27" s="1">
+        <v>34</v>
+      </c>
+      <c r="E27" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>21</v>
+      </c>
+      <c r="B28" s="2">
+        <v>1127.9000000000001</v>
+      </c>
+      <c r="C28">
+        <v>2</v>
+      </c>
+      <c r="D28" s="1">
+        <v>22.9</v>
+      </c>
+      <c r="E28" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>22</v>
+      </c>
+      <c r="B29" s="2">
+        <v>1127.9000000000001</v>
+      </c>
+      <c r="D29" s="1">
+        <v>28.3</v>
+      </c>
+      <c r="E29" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>23</v>
+      </c>
+      <c r="B30" s="2">
+        <v>1127.9000000000001</v>
+      </c>
+      <c r="D30" s="1">
+        <v>32.700000000000003</v>
+      </c>
+      <c r="E30" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>24</v>
+      </c>
+      <c r="B31" s="2">
+        <v>1140.4000000000001</v>
+      </c>
+      <c r="C31">
+        <v>2</v>
+      </c>
+      <c r="D31" s="1">
+        <v>22</v>
+      </c>
+      <c r="E31" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>25</v>
+      </c>
+      <c r="B32" s="2">
+        <v>1140.4000000000001</v>
+      </c>
+      <c r="D32" s="1">
+        <v>24.1</v>
+      </c>
+      <c r="E32" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>26</v>
+      </c>
+      <c r="B33" s="2">
+        <v>1140.4000000000001</v>
+      </c>
+      <c r="D33" s="1">
+        <v>28.8</v>
+      </c>
+      <c r="E33" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>27</v>
+      </c>
+      <c r="B34" s="2">
+        <v>1148.4000000000001</v>
+      </c>
+      <c r="C34">
+        <v>2</v>
+      </c>
+      <c r="D34" s="1">
+        <v>26.6</v>
+      </c>
+      <c r="E34" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>28</v>
+      </c>
+      <c r="B35" s="2">
+        <v>1148.4000000000001</v>
+      </c>
+      <c r="D35" s="1">
+        <v>28.6</v>
+      </c>
+      <c r="E35" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>29</v>
+      </c>
+      <c r="B36" s="2">
+        <v>1148.4000000000001</v>
+      </c>
+      <c r="D36" s="1">
+        <v>32.4</v>
+      </c>
+      <c r="E36" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>30</v>
+      </c>
+      <c r="B37" s="2">
+        <v>1148.4000000000001</v>
+      </c>
+      <c r="D37" s="1">
+        <v>35.1</v>
+      </c>
+      <c r="E37" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>31</v>
+      </c>
+      <c r="B38" s="2">
+        <v>1182.3</v>
+      </c>
+      <c r="C38">
+        <v>2</v>
+      </c>
+      <c r="D38" s="1">
+        <v>23.9</v>
+      </c>
+      <c r="E38" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>32</v>
+      </c>
+      <c r="B39" s="2">
+        <v>1184.4000000000001</v>
+      </c>
+      <c r="C39">
+        <v>2</v>
+      </c>
+      <c r="D39" s="1">
+        <v>34.5</v>
+      </c>
+      <c r="E39" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>33</v>
+      </c>
+      <c r="B40" s="2">
+        <v>1184.4000000000001</v>
+      </c>
+      <c r="D40" s="1">
+        <v>42.2</v>
+      </c>
+      <c r="E40" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>34</v>
+      </c>
+      <c r="B41" s="2">
+        <v>1184.4000000000001</v>
+      </c>
+      <c r="D41" s="1">
+        <v>48.4</v>
+      </c>
+      <c r="E41" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>35</v>
+      </c>
+      <c r="B42" s="2">
+        <v>1195.4000000000001</v>
+      </c>
+      <c r="C42">
+        <v>2</v>
+      </c>
+      <c r="D42" s="1">
+        <v>34.200000000000003</v>
+      </c>
+      <c r="E42" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>36</v>
+      </c>
+      <c r="B43" s="2">
+        <v>1200.9000000000001</v>
+      </c>
+      <c r="C43">
+        <v>2</v>
+      </c>
+      <c r="D43" s="1">
+        <v>27.4</v>
+      </c>
+      <c r="E43" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>37</v>
+      </c>
+      <c r="B44" s="2">
+        <v>1212.9000000000001</v>
+      </c>
+      <c r="C44">
+        <v>2</v>
+      </c>
+      <c r="D44" s="1">
+        <v>27.9</v>
+      </c>
+      <c r="E44" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>38</v>
+      </c>
+      <c r="B45" s="2">
+        <v>1212.9000000000001</v>
+      </c>
+      <c r="D45" s="1">
+        <v>35.4</v>
+      </c>
+      <c r="E45" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>39</v>
+      </c>
+      <c r="B46" s="2">
+        <v>1221.4000000000001</v>
+      </c>
+      <c r="C46">
+        <v>2</v>
+      </c>
+      <c r="D46" s="1">
+        <v>27.2</v>
+      </c>
+      <c r="E46" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>40</v>
+      </c>
+      <c r="B47" s="2">
+        <v>1221.4000000000001</v>
+      </c>
+      <c r="D47" s="1">
+        <v>30.5</v>
+      </c>
+      <c r="E47" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>41</v>
+      </c>
+      <c r="B48" s="2">
+        <v>1221.4000000000001</v>
+      </c>
+      <c r="D48" s="1">
+        <v>32.9</v>
+      </c>
+      <c r="E48" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>42</v>
+      </c>
+      <c r="B49" s="2">
+        <v>1221.4000000000001</v>
+      </c>
+      <c r="D49" s="1">
+        <v>34.700000000000003</v>
+      </c>
+      <c r="E49" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>43</v>
+      </c>
+      <c r="B50" s="2">
+        <v>1221.4000000000001</v>
+      </c>
+      <c r="D50" s="1">
+        <v>36.9</v>
+      </c>
+      <c r="E50" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>44</v>
+      </c>
+      <c r="B51" s="2">
+        <v>1221.4000000000001</v>
+      </c>
+      <c r="D51" s="1">
+        <v>39.200000000000003</v>
+      </c>
+      <c r="E51" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>45</v>
+      </c>
+      <c r="B52" s="2">
+        <v>1229.5</v>
+      </c>
+      <c r="C52">
+        <v>2</v>
+      </c>
+      <c r="D52" s="1">
+        <v>20.3</v>
+      </c>
+      <c r="E52" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>46</v>
+      </c>
+      <c r="B53" s="2">
+        <v>1229.5</v>
+      </c>
+      <c r="D53" s="1">
+        <v>23.3</v>
+      </c>
+      <c r="E53" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>47</v>
+      </c>
+      <c r="B54" s="2">
+        <v>1235.5</v>
+      </c>
+      <c r="C54">
+        <v>1</v>
+      </c>
+      <c r="D54" s="1">
+        <v>26.2</v>
+      </c>
+      <c r="E54" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>48</v>
+      </c>
+      <c r="B55" s="2">
+        <v>1235.5</v>
+      </c>
+      <c r="D55" s="1">
+        <v>27.9</v>
+      </c>
+      <c r="E55" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>49</v>
+      </c>
+      <c r="B56" s="2">
+        <v>1250</v>
+      </c>
+      <c r="C56">
+        <v>2</v>
+      </c>
+      <c r="D56" s="1">
+        <v>21.5</v>
+      </c>
+      <c r="E56" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>50</v>
+      </c>
+      <c r="B57" s="2">
+        <v>1250</v>
+      </c>
+      <c r="D57" s="1">
+        <v>23.5</v>
+      </c>
+      <c r="E57" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>51</v>
+      </c>
+      <c r="B58" s="2">
+        <v>1286</v>
+      </c>
+      <c r="C58">
+        <v>2</v>
+      </c>
+      <c r="D58" s="1">
+        <v>27.1</v>
+      </c>
+      <c r="E58" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>52</v>
+      </c>
+      <c r="B59" s="2">
+        <v>1286</v>
+      </c>
+      <c r="D59" s="1">
+        <v>32.1</v>
+      </c>
+      <c r="E59" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>53</v>
+      </c>
+      <c r="B60" s="2">
+        <v>1286</v>
+      </c>
+      <c r="D60" s="1">
+        <v>39.1</v>
+      </c>
+      <c r="E60" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>54</v>
+      </c>
+      <c r="B61" s="2">
+        <v>1323</v>
+      </c>
+      <c r="C61">
+        <v>2</v>
+      </c>
+      <c r="D61" s="1">
+        <v>25.6</v>
+      </c>
+      <c r="E61" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>55</v>
+      </c>
+      <c r="B62" s="2">
+        <v>1323</v>
+      </c>
+      <c r="D62" s="1">
+        <v>27.1</v>
+      </c>
+      <c r="E62" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>56</v>
+      </c>
+      <c r="B63" s="2">
+        <v>1323</v>
+      </c>
+      <c r="D63" s="1">
+        <v>28.2</v>
+      </c>
+      <c r="E63" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>57</v>
+      </c>
+      <c r="B64" s="2">
+        <v>1323</v>
+      </c>
+      <c r="D64" s="1">
+        <v>29.8</v>
+      </c>
+      <c r="E64" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>58</v>
+      </c>
+      <c r="B65" s="2">
+        <v>1323</v>
+      </c>
+      <c r="D65" s="1">
+        <v>31.8</v>
+      </c>
+      <c r="E65" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>59</v>
+      </c>
+      <c r="B66" s="2">
+        <v>1331</v>
+      </c>
+      <c r="C66">
+        <v>2</v>
+      </c>
+      <c r="D66" s="1">
+        <v>33.6</v>
+      </c>
+      <c r="E66" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>60</v>
+      </c>
+      <c r="B67" s="2">
+        <v>1366.9</v>
+      </c>
+      <c r="C67">
+        <v>2</v>
+      </c>
+      <c r="D67" s="1">
+        <v>32.9</v>
+      </c>
+      <c r="E67" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>61</v>
+      </c>
+      <c r="B68" s="2">
+        <v>1366.9</v>
+      </c>
+      <c r="D68" s="1">
+        <v>37.799999999999997</v>
+      </c>
+      <c r="E68" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>62</v>
+      </c>
+      <c r="B69" s="2">
+        <v>1366.9</v>
+      </c>
+      <c r="D69" s="1">
+        <v>39.1</v>
+      </c>
+      <c r="E69" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>63</v>
+      </c>
+      <c r="B70" s="2">
+        <v>1366.9</v>
+      </c>
+      <c r="D70" s="1">
+        <v>42</v>
+      </c>
+      <c r="E70" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>64</v>
+      </c>
+      <c r="B71" s="2">
+        <v>1366.9</v>
+      </c>
+      <c r="D71" s="1">
+        <v>45</v>
+      </c>
+      <c r="E71" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>65</v>
+      </c>
+      <c r="B72" s="2">
+        <v>1366.9</v>
+      </c>
+      <c r="D72" s="1">
+        <v>46.5</v>
+      </c>
+      <c r="E72" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>66</v>
+      </c>
+      <c r="B73" s="2">
+        <v>1366.9</v>
+      </c>
+      <c r="D73" s="1">
+        <v>47.8</v>
+      </c>
+      <c r="E73" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>67</v>
+      </c>
+      <c r="B74" s="2">
+        <v>1367</v>
+      </c>
+      <c r="C74">
+        <v>2</v>
+      </c>
+      <c r="D74" s="1">
+        <v>38</v>
+      </c>
+      <c r="E74" s="1">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>68</v>
+      </c>
+      <c r="B75" s="2">
+        <v>1367</v>
+      </c>
+      <c r="D75" s="1">
+        <v>38.799999999999997</v>
+      </c>
+      <c r="E75" s="1">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>69</v>
+      </c>
+      <c r="B76" s="2">
+        <v>1367</v>
+      </c>
+      <c r="D76" s="1">
+        <v>41.6</v>
+      </c>
+      <c r="E76" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>70</v>
+      </c>
+      <c r="B77" s="2">
+        <v>1367</v>
+      </c>
+      <c r="D77" s="1">
+        <v>42.6</v>
+      </c>
+      <c r="E77" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>71</v>
+      </c>
+      <c r="B78" s="2">
+        <v>1367</v>
+      </c>
+      <c r="D78" s="1">
+        <v>45</v>
+      </c>
+      <c r="E78" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>72</v>
+      </c>
+      <c r="B79" s="2">
+        <v>1367</v>
+      </c>
+      <c r="D79" s="1">
+        <v>46.5</v>
+      </c>
+      <c r="E79" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>73</v>
+      </c>
+      <c r="B80" s="2">
+        <v>1367</v>
+      </c>
+      <c r="D80" s="1">
+        <v>47.8</v>
+      </c>
+      <c r="E80" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>74</v>
+      </c>
+      <c r="B81" s="2">
+        <v>1367</v>
+      </c>
+      <c r="D81" s="1">
+        <v>48.9</v>
+      </c>
+      <c r="E81" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>75</v>
+      </c>
+      <c r="B82" s="2">
+        <v>1367</v>
+      </c>
+      <c r="D82" s="1">
+        <v>51</v>
+      </c>
+      <c r="E82" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>76</v>
+      </c>
+      <c r="B83" s="2">
+        <v>1404</v>
+      </c>
+      <c r="C83">
+        <v>2</v>
+      </c>
+      <c r="D83" s="1">
+        <v>30.3</v>
+      </c>
+      <c r="E83" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>77</v>
+      </c>
+      <c r="B84" s="2">
+        <v>1404</v>
+      </c>
+      <c r="D84" s="1">
+        <v>33</v>
+      </c>
+      <c r="E84" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>78</v>
+      </c>
+      <c r="B85" s="2">
+        <v>1404</v>
+      </c>
+      <c r="D85" s="1">
+        <v>37.1</v>
+      </c>
+      <c r="E85" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>79</v>
+      </c>
+      <c r="B86" s="2">
+        <v>1422</v>
+      </c>
+      <c r="C86">
+        <v>2</v>
+      </c>
+      <c r="D86" s="1">
+        <v>37.200000000000003</v>
+      </c>
+      <c r="E86" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>80</v>
+      </c>
+      <c r="B87" s="2">
+        <v>1468.5</v>
+      </c>
+      <c r="C87">
+        <v>2</v>
+      </c>
+      <c r="D87" s="1">
+        <v>28.7</v>
+      </c>
+      <c r="E87" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>81</v>
+      </c>
+      <c r="B88" s="2">
+        <v>1468.5</v>
+      </c>
+      <c r="D88" s="1">
+        <v>30.6</v>
+      </c>
+      <c r="E88" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>82</v>
+      </c>
+      <c r="B89" s="2">
+        <v>1468.5</v>
+      </c>
+      <c r="D89" s="1">
+        <v>32.200000000000003</v>
+      </c>
+      <c r="E89" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <v>83</v>
+      </c>
+      <c r="B90" s="2">
+        <v>1468.5</v>
+      </c>
+      <c r="D90" s="1">
+        <v>34.299999999999997</v>
+      </c>
+      <c r="E90" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <v>84</v>
+      </c>
+      <c r="B91" s="2">
+        <v>1468.5</v>
+      </c>
+      <c r="D91" s="1">
+        <v>41.9</v>
+      </c>
+      <c r="E91" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <v>85</v>
+      </c>
+      <c r="B92" s="2">
+        <v>1468.5</v>
+      </c>
+      <c r="D92" s="1">
+        <v>46.6</v>
+      </c>
+      <c r="E92" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <v>86</v>
+      </c>
+      <c r="B93" s="2">
+        <v>1505.5</v>
+      </c>
+      <c r="C93">
+        <v>2</v>
+      </c>
+      <c r="D93" s="1">
+        <v>23.2</v>
+      </c>
+      <c r="E93" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A94">
+        <v>87</v>
+      </c>
+      <c r="B94" s="2">
+        <v>1505.5</v>
+      </c>
+      <c r="D94" s="1">
+        <v>28.1</v>
+      </c>
+      <c r="E94" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A95">
+        <v>88</v>
+      </c>
+      <c r="B95" s="2">
+        <v>1505.5</v>
+      </c>
+      <c r="D95" s="1">
+        <v>30.7</v>
+      </c>
+      <c r="E95" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A96">
+        <v>89</v>
+      </c>
+      <c r="B96" s="2">
+        <v>1505.5</v>
+      </c>
+      <c r="D96" s="1">
+        <v>32.1</v>
+      </c>
+      <c r="E96" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A97">
+        <v>90</v>
+      </c>
+      <c r="B97" s="2">
+        <v>1513.5</v>
+      </c>
+      <c r="C97">
+        <v>2</v>
+      </c>
+      <c r="D97" s="1">
+        <v>35.4</v>
+      </c>
+      <c r="E97" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A98">
+        <v>91</v>
+      </c>
+      <c r="B98" s="2">
+        <v>1586.5</v>
+      </c>
+      <c r="C98">
+        <v>2</v>
+      </c>
+      <c r="D98" s="1">
+        <v>39.799999999999997</v>
+      </c>
+      <c r="E98" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A99">
+        <v>92</v>
+      </c>
+      <c r="B99" s="2">
+        <v>1651</v>
+      </c>
+      <c r="C99">
+        <v>2</v>
+      </c>
+      <c r="D99" s="1">
+        <v>34.1</v>
+      </c>
+      <c r="E99" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A100">
+        <v>93</v>
+      </c>
+      <c r="B100" s="2">
+        <v>1651</v>
+      </c>
+      <c r="D100" s="1">
+        <v>44.2</v>
+      </c>
+      <c r="E100" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A101">
+        <v>100</v>
+      </c>
+      <c r="B101" s="2">
+        <v>739.3</v>
+      </c>
+      <c r="C101">
+        <v>2</v>
+      </c>
+      <c r="D101" s="1">
+        <v>13</v>
+      </c>
+      <c r="E101" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A102">
+        <v>101</v>
+      </c>
+      <c r="B102" s="2">
+        <v>759.8</v>
+      </c>
+      <c r="C102">
+        <v>2</v>
+      </c>
+      <c r="D102" s="1">
+        <v>13.5</v>
+      </c>
+      <c r="E102" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A103">
+        <v>102</v>
+      </c>
+      <c r="B103" s="2">
+        <v>779.3</v>
+      </c>
+      <c r="C103">
+        <v>2</v>
+      </c>
+      <c r="D103" s="1">
+        <v>18.600000000000001</v>
+      </c>
+      <c r="E103" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A104">
+        <v>103</v>
+      </c>
+      <c r="B104" s="2">
+        <v>779.3</v>
+      </c>
+      <c r="D104" s="1">
+        <v>19.8</v>
+      </c>
+      <c r="E104" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A105">
+        <v>104</v>
+      </c>
+      <c r="B105" s="2">
+        <v>799.8</v>
+      </c>
+      <c r="C105">
+        <v>2</v>
+      </c>
+      <c r="D105" s="1">
+        <v>22.5</v>
+      </c>
+      <c r="E105" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A106">
+        <v>105</v>
+      </c>
+      <c r="B106" s="2">
+        <v>820.3</v>
+      </c>
+      <c r="C106">
+        <v>2</v>
+      </c>
+      <c r="D106" s="1">
+        <v>13.9</v>
+      </c>
+      <c r="E106" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A107">
+        <v>106</v>
+      </c>
+      <c r="B107" s="2">
+        <v>820.3</v>
+      </c>
+      <c r="D107" s="1">
+        <v>16.2</v>
+      </c>
+      <c r="E107" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A108">
+        <v>107</v>
+      </c>
+      <c r="B108" s="2">
+        <v>820.3</v>
+      </c>
+      <c r="D108" s="1">
+        <v>24.2</v>
+      </c>
+      <c r="E108" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A109">
+        <v>108</v>
+      </c>
+      <c r="B109" s="2">
+        <v>832.8</v>
+      </c>
+      <c r="C109">
+        <v>2</v>
+      </c>
+      <c r="D109" s="1">
+        <v>18.2</v>
+      </c>
+      <c r="E109" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A110">
+        <v>109</v>
+      </c>
+      <c r="B110" s="2">
+        <v>832.8</v>
+      </c>
+      <c r="D110" s="1">
+        <v>23.7</v>
+      </c>
+      <c r="E110" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A111">
+        <v>110</v>
+      </c>
+      <c r="B111" s="2">
+        <v>840.8</v>
+      </c>
+      <c r="C111">
+        <v>2</v>
+      </c>
+      <c r="D111" s="1">
+        <v>14.7</v>
+      </c>
+      <c r="E111" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A112">
+        <v>111</v>
+      </c>
+      <c r="B112" s="2">
+        <v>840.8</v>
+      </c>
+      <c r="D112" s="1">
+        <v>15.4</v>
+      </c>
+      <c r="E112" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A113">
+        <v>112</v>
+      </c>
+      <c r="B113" s="2">
+        <v>860.3</v>
+      </c>
+      <c r="C113">
+        <v>2</v>
+      </c>
+      <c r="D113" s="1">
+        <v>15.3</v>
+      </c>
+      <c r="E113" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A114">
+        <v>113</v>
+      </c>
+      <c r="B114" s="2">
+        <v>860.3</v>
+      </c>
+      <c r="D114" s="1">
+        <v>18.600000000000001</v>
+      </c>
+      <c r="E114" s="1">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A115">
+        <v>114</v>
+      </c>
+      <c r="B115" s="2">
+        <v>860.3</v>
+      </c>
+      <c r="D115" s="1">
+        <v>19.600000000000001</v>
+      </c>
+      <c r="E115" s="1">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A116">
+        <v>115</v>
+      </c>
+      <c r="B116" s="2">
+        <v>860.3</v>
+      </c>
+      <c r="D116" s="1">
+        <v>20.2</v>
+      </c>
+      <c r="E116" s="1">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A117">
+        <v>116</v>
+      </c>
+      <c r="B117" s="2">
+        <v>860.3</v>
+      </c>
+      <c r="D117" s="1">
+        <v>22.3</v>
+      </c>
+      <c r="E117" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A118">
+        <v>117</v>
+      </c>
+      <c r="B118" s="2">
+        <v>864.3</v>
+      </c>
+      <c r="C118">
+        <v>2</v>
+      </c>
+      <c r="D118" s="1">
+        <v>22.8</v>
+      </c>
+      <c r="E118" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A119">
+        <v>118</v>
+      </c>
+      <c r="B119" s="2">
+        <v>867.3</v>
+      </c>
+      <c r="C119">
+        <v>2</v>
+      </c>
+      <c r="D119" s="1">
+        <v>29.7</v>
+      </c>
+      <c r="E119" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A120">
+        <v>119</v>
+      </c>
+      <c r="B120" s="2">
+        <v>893.3</v>
+      </c>
+      <c r="C120">
+        <v>2</v>
+      </c>
+      <c r="D120" s="1">
+        <v>20.7</v>
+      </c>
+      <c r="E120" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A121">
+        <v>120</v>
+      </c>
+      <c r="B121" s="2">
+        <v>893.3</v>
+      </c>
+      <c r="D121" s="1">
+        <v>29.7</v>
+      </c>
+      <c r="E121" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A122">
+        <v>121</v>
+      </c>
+      <c r="B122" s="2">
+        <v>901.4</v>
+      </c>
+      <c r="C122">
+        <v>2</v>
+      </c>
+      <c r="D122" s="1">
+        <v>14.7</v>
+      </c>
+      <c r="E122" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A123">
+        <v>122</v>
+      </c>
+      <c r="B123" s="2">
+        <v>901.4</v>
+      </c>
+      <c r="D123" s="1">
+        <v>17.7</v>
+      </c>
+      <c r="E123" s="1">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A124">
+        <v>123</v>
+      </c>
+      <c r="B124" s="2">
+        <v>901.4</v>
+      </c>
+      <c r="D124" s="1">
+        <v>18.2</v>
+      </c>
+      <c r="E124" s="1">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A125">
+        <v>124</v>
+      </c>
+      <c r="B125" s="2">
+        <v>913.9</v>
+      </c>
+      <c r="C125">
+        <v>2</v>
+      </c>
+      <c r="D125" s="1">
+        <v>18.7</v>
+      </c>
+      <c r="E125" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A126">
+        <v>125</v>
+      </c>
+      <c r="B126" s="2">
+        <v>913.9</v>
+      </c>
+      <c r="D126" s="1">
+        <v>20.100000000000001</v>
+      </c>
+      <c r="E126" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A127">
+        <v>126</v>
+      </c>
+      <c r="B127" s="2">
+        <v>921.9</v>
+      </c>
+      <c r="C127">
+        <v>2</v>
+      </c>
+      <c r="D127" s="1">
+        <v>16.5</v>
+      </c>
+      <c r="E127" s="1">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A128">
+        <v>127</v>
+      </c>
+      <c r="B128" s="2">
+        <v>937.4</v>
+      </c>
+      <c r="C128">
+        <v>2</v>
+      </c>
+      <c r="D128" s="1">
+        <v>27.8</v>
+      </c>
+      <c r="E128" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A129">
+        <v>128</v>
+      </c>
+      <c r="B129" s="2">
+        <v>941.3</v>
+      </c>
+      <c r="C129">
+        <v>2</v>
+      </c>
+      <c r="D129" s="1">
+        <v>15.6</v>
+      </c>
+      <c r="E129" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A130">
+        <v>129</v>
+      </c>
+      <c r="B130" s="2">
+        <v>941.3</v>
+      </c>
+      <c r="D130" s="1">
+        <v>18.899999999999999</v>
+      </c>
+      <c r="E130" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A131">
+        <v>130</v>
+      </c>
+      <c r="B131" s="2">
+        <v>941.3</v>
+      </c>
+      <c r="D131" s="1">
+        <v>20.100000000000001</v>
+      </c>
+      <c r="E131" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A132">
+        <v>131</v>
+      </c>
+      <c r="B132" s="2">
+        <v>945.4</v>
+      </c>
+      <c r="C132">
+        <v>2</v>
+      </c>
+      <c r="D132" s="1">
+        <v>25.6</v>
+      </c>
+      <c r="E132" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A133">
+        <v>132</v>
+      </c>
+      <c r="B133" s="2">
+        <v>945.4</v>
+      </c>
+      <c r="D133" s="1">
+        <v>33.5</v>
+      </c>
+      <c r="E133" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A134">
+        <v>133</v>
+      </c>
+      <c r="B134" s="2">
+        <v>957.9</v>
+      </c>
+      <c r="C134">
+        <v>2</v>
+      </c>
+      <c r="D134" s="1">
+        <v>30.3</v>
+      </c>
+      <c r="E134" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A135">
+        <v>134</v>
+      </c>
+      <c r="B135" s="2">
+        <v>965.9</v>
+      </c>
+      <c r="C135">
+        <v>2</v>
+      </c>
+      <c r="D135" s="1">
+        <v>22.6</v>
+      </c>
+      <c r="E135" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A136">
+        <v>135</v>
+      </c>
+      <c r="B136" s="2">
+        <v>965.9</v>
+      </c>
+      <c r="D136" s="1">
+        <v>27.2</v>
+      </c>
+      <c r="E136" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A137">
+        <v>136</v>
+      </c>
+      <c r="B137" s="2">
+        <v>965.9</v>
+      </c>
+      <c r="D137" s="1">
+        <v>31.5</v>
+      </c>
+      <c r="E137" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A138">
+        <v>137</v>
+      </c>
+      <c r="B138" s="2">
+        <v>965.9</v>
+      </c>
+      <c r="D138" s="1">
+        <v>35.700000000000003</v>
+      </c>
+      <c r="E138" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A139">
+        <v>138</v>
+      </c>
+      <c r="B139" s="2">
+        <v>974.4</v>
+      </c>
+      <c r="C139">
+        <v>2</v>
+      </c>
+      <c r="D139" s="1">
+        <v>22</v>
+      </c>
+      <c r="E139" s="1">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A140">
+        <v>139</v>
+      </c>
+      <c r="B140" s="2">
+        <v>974.4</v>
+      </c>
+      <c r="D140" s="1">
+        <v>22.9</v>
+      </c>
+      <c r="E140" s="1">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A141">
+        <v>140</v>
+      </c>
+      <c r="B141" s="2">
+        <v>982.3</v>
+      </c>
+      <c r="C141">
+        <v>2</v>
+      </c>
+      <c r="D141" s="1">
+        <v>16.3</v>
+      </c>
+      <c r="E141" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A142">
+        <v>141</v>
+      </c>
+      <c r="B142" s="2">
+        <v>982.3</v>
+      </c>
+      <c r="D142" s="1">
+        <v>19.399999999999999</v>
+      </c>
+      <c r="E142" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A143">
+        <v>142</v>
+      </c>
+      <c r="B143" s="2">
+        <v>994.9</v>
+      </c>
+      <c r="C143">
+        <v>2</v>
+      </c>
+      <c r="D143" s="1">
+        <v>21</v>
+      </c>
+      <c r="E143" s="1">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updates example data for QuantAnalysis_Method_Writer
</commit_message>
<xml_diff>
--- a/QuantAnalysis/example_data_EIC_RT.xlsx
+++ b/QuantAnalysis/example_data_EIC_RT.xlsx
@@ -4,18 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="45" windowWidth="20115" windowHeight="11310" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="45" windowWidth="20115" windowHeight="11310" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="5" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="6" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="7" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="12">
   <si>
     <t>1; 2</t>
   </si>
@@ -2167,7 +2168,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E143"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I120" sqref="I120"/>
     </sheetView>
   </sheetViews>
@@ -4357,4 +4358,2203 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E143"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H91" sqref="H91"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="16.5703125" customWidth="1"/>
+    <col min="3" max="3" width="8.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>67</v>
+      </c>
+      <c r="B2" s="2">
+        <v>1367</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+      <c r="D2" s="1">
+        <v>38</v>
+      </c>
+      <c r="E2" s="1">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>68</v>
+      </c>
+      <c r="B3" s="2">
+        <v>1367</v>
+      </c>
+      <c r="D3" s="1">
+        <v>38.799999999999997</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>69</v>
+      </c>
+      <c r="B4" s="2">
+        <v>1367</v>
+      </c>
+      <c r="D4" s="1">
+        <v>41.6</v>
+      </c>
+      <c r="E4" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>70</v>
+      </c>
+      <c r="B5" s="2">
+        <v>1367</v>
+      </c>
+      <c r="D5" s="1">
+        <v>42.6</v>
+      </c>
+      <c r="E5" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>71</v>
+      </c>
+      <c r="B6" s="2">
+        <v>1367</v>
+      </c>
+      <c r="D6" s="1">
+        <v>45</v>
+      </c>
+      <c r="E6" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>72</v>
+      </c>
+      <c r="B7" s="2">
+        <v>1367</v>
+      </c>
+      <c r="D7" s="1">
+        <v>46.5</v>
+      </c>
+      <c r="E7" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>73</v>
+      </c>
+      <c r="B8" s="2">
+        <v>1367</v>
+      </c>
+      <c r="D8" s="1">
+        <v>47.8</v>
+      </c>
+      <c r="E8" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>74</v>
+      </c>
+      <c r="B9" s="2">
+        <v>1367</v>
+      </c>
+      <c r="D9" s="1">
+        <v>48.9</v>
+      </c>
+      <c r="E9" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>75</v>
+      </c>
+      <c r="B10" s="2">
+        <v>1367</v>
+      </c>
+      <c r="D10" s="1">
+        <v>51</v>
+      </c>
+      <c r="E10" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>76</v>
+      </c>
+      <c r="B11" s="2">
+        <v>1404</v>
+      </c>
+      <c r="C11">
+        <v>2</v>
+      </c>
+      <c r="D11" s="1">
+        <v>30.3</v>
+      </c>
+      <c r="E11" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>77</v>
+      </c>
+      <c r="B12" s="2">
+        <v>1404</v>
+      </c>
+      <c r="D12" s="1">
+        <v>33</v>
+      </c>
+      <c r="E12" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>78</v>
+      </c>
+      <c r="B13" s="2">
+        <v>1404</v>
+      </c>
+      <c r="D13" s="1">
+        <v>37.1</v>
+      </c>
+      <c r="E13" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>79</v>
+      </c>
+      <c r="B14" s="2">
+        <v>1422</v>
+      </c>
+      <c r="C14">
+        <v>2</v>
+      </c>
+      <c r="D14" s="1">
+        <v>37.200000000000003</v>
+      </c>
+      <c r="E14" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>80</v>
+      </c>
+      <c r="B15" s="2">
+        <v>1468.5</v>
+      </c>
+      <c r="C15">
+        <v>2</v>
+      </c>
+      <c r="D15" s="1">
+        <v>28.7</v>
+      </c>
+      <c r="E15" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>81</v>
+      </c>
+      <c r="B16" s="2">
+        <v>1468.5</v>
+      </c>
+      <c r="D16" s="1">
+        <v>30.6</v>
+      </c>
+      <c r="E16" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>82</v>
+      </c>
+      <c r="B17" s="2">
+        <v>1468.5</v>
+      </c>
+      <c r="D17" s="1">
+        <v>32.200000000000003</v>
+      </c>
+      <c r="E17" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>83</v>
+      </c>
+      <c r="B18" s="2">
+        <v>1468.5</v>
+      </c>
+      <c r="D18" s="1">
+        <v>34.299999999999997</v>
+      </c>
+      <c r="E18" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>84</v>
+      </c>
+      <c r="B19" s="2">
+        <v>1468.5</v>
+      </c>
+      <c r="D19" s="1">
+        <v>41.9</v>
+      </c>
+      <c r="E19" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>85</v>
+      </c>
+      <c r="B20" s="2">
+        <v>1468.5</v>
+      </c>
+      <c r="D20" s="1">
+        <v>46.6</v>
+      </c>
+      <c r="E20" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>86</v>
+      </c>
+      <c r="B21" s="2">
+        <v>1505.5</v>
+      </c>
+      <c r="C21">
+        <v>2</v>
+      </c>
+      <c r="D21" s="1">
+        <v>23.2</v>
+      </c>
+      <c r="E21" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>87</v>
+      </c>
+      <c r="B22" s="2">
+        <v>1505.5</v>
+      </c>
+      <c r="D22" s="1">
+        <v>28.1</v>
+      </c>
+      <c r="E22" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>88</v>
+      </c>
+      <c r="B23" s="2">
+        <v>1505.5</v>
+      </c>
+      <c r="D23" s="1">
+        <v>30.7</v>
+      </c>
+      <c r="E23" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>89</v>
+      </c>
+      <c r="B24" s="2">
+        <v>1505.5</v>
+      </c>
+      <c r="D24" s="1">
+        <v>32.1</v>
+      </c>
+      <c r="E24" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>90</v>
+      </c>
+      <c r="B25" s="2">
+        <v>1513.5</v>
+      </c>
+      <c r="C25">
+        <v>2</v>
+      </c>
+      <c r="D25" s="1">
+        <v>35.4</v>
+      </c>
+      <c r="E25" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>91</v>
+      </c>
+      <c r="B26" s="2">
+        <v>1586.5</v>
+      </c>
+      <c r="C26">
+        <v>2</v>
+      </c>
+      <c r="D26" s="1">
+        <v>39.799999999999997</v>
+      </c>
+      <c r="E26" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>92</v>
+      </c>
+      <c r="B27" s="2">
+        <v>1651</v>
+      </c>
+      <c r="C27">
+        <v>2</v>
+      </c>
+      <c r="D27" s="1">
+        <v>34.1</v>
+      </c>
+      <c r="E27" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>93</v>
+      </c>
+      <c r="B28" s="2">
+        <v>1651</v>
+      </c>
+      <c r="D28" s="1">
+        <v>44.2</v>
+      </c>
+      <c r="E28" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>1</v>
+      </c>
+      <c r="B29" s="2">
+        <v>1018.4</v>
+      </c>
+      <c r="C29">
+        <v>2</v>
+      </c>
+      <c r="D29" s="1">
+        <v>30.6</v>
+      </c>
+      <c r="E29" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>2</v>
+      </c>
+      <c r="B30" s="2">
+        <v>1022.4</v>
+      </c>
+      <c r="C30">
+        <v>2</v>
+      </c>
+      <c r="D30" s="1">
+        <v>20.5</v>
+      </c>
+      <c r="E30" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>3</v>
+      </c>
+      <c r="B31" s="2">
+        <v>1038.9000000000001</v>
+      </c>
+      <c r="C31">
+        <v>2</v>
+      </c>
+      <c r="D31" s="1">
+        <v>29</v>
+      </c>
+      <c r="E31" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>4</v>
+      </c>
+      <c r="B32" s="2">
+        <v>1038.9000000000001</v>
+      </c>
+      <c r="D32" s="1">
+        <v>32.1</v>
+      </c>
+      <c r="E32" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>5</v>
+      </c>
+      <c r="B33" s="2">
+        <v>1038.9000000000001</v>
+      </c>
+      <c r="D33" s="1">
+        <v>35</v>
+      </c>
+      <c r="E33" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>6</v>
+      </c>
+      <c r="B34" s="2">
+        <v>1038.9000000000001</v>
+      </c>
+      <c r="D34" s="1">
+        <v>36.5</v>
+      </c>
+      <c r="E34" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>7</v>
+      </c>
+      <c r="B35" s="2">
+        <v>1038.9000000000001</v>
+      </c>
+      <c r="D35" s="1">
+        <v>39.799999999999997</v>
+      </c>
+      <c r="E35" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>8</v>
+      </c>
+      <c r="B36" s="2">
+        <v>1046.9000000000001</v>
+      </c>
+      <c r="C36">
+        <v>2</v>
+      </c>
+      <c r="D36" s="1">
+        <v>17.5</v>
+      </c>
+      <c r="E36" s="1">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>9</v>
+      </c>
+      <c r="B37" s="2">
+        <v>1046.9000000000001</v>
+      </c>
+      <c r="D37" s="1">
+        <v>21.3</v>
+      </c>
+      <c r="E37" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>10</v>
+      </c>
+      <c r="B38" s="2">
+        <v>1046.9000000000001</v>
+      </c>
+      <c r="D38" s="1">
+        <v>29.9</v>
+      </c>
+      <c r="E38" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>11</v>
+      </c>
+      <c r="B39" s="2">
+        <v>1059.4000000000001</v>
+      </c>
+      <c r="C39">
+        <v>2</v>
+      </c>
+      <c r="D39" s="1">
+        <v>22.3</v>
+      </c>
+      <c r="E39" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>12</v>
+      </c>
+      <c r="B40" s="2">
+        <v>1067.4000000000001</v>
+      </c>
+      <c r="C40">
+        <v>2</v>
+      </c>
+      <c r="D40" s="1">
+        <v>19.899999999999999</v>
+      </c>
+      <c r="E40" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>13</v>
+      </c>
+      <c r="B41" s="2">
+        <v>1067.4000000000001</v>
+      </c>
+      <c r="D41" s="1">
+        <v>25.1</v>
+      </c>
+      <c r="E41" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>14</v>
+      </c>
+      <c r="B42" s="2">
+        <v>1083.9000000000001</v>
+      </c>
+      <c r="C42">
+        <v>2</v>
+      </c>
+      <c r="D42" s="1">
+        <v>20.399999999999999</v>
+      </c>
+      <c r="E42" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>15</v>
+      </c>
+      <c r="B43" s="2">
+        <v>1111.4000000000001</v>
+      </c>
+      <c r="C43">
+        <v>2</v>
+      </c>
+      <c r="D43" s="1">
+        <v>29.7</v>
+      </c>
+      <c r="E43" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>16</v>
+      </c>
+      <c r="B44" s="2">
+        <v>1111.4000000000001</v>
+      </c>
+      <c r="D44" s="1">
+        <v>37.700000000000003</v>
+      </c>
+      <c r="E44" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>17</v>
+      </c>
+      <c r="B45" s="2">
+        <v>1111.4000000000001</v>
+      </c>
+      <c r="D45" s="1">
+        <v>44.2</v>
+      </c>
+      <c r="E45" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>18</v>
+      </c>
+      <c r="B46" s="2">
+        <v>1119.9000000000001</v>
+      </c>
+      <c r="C46">
+        <v>2</v>
+      </c>
+      <c r="D46" s="1">
+        <v>21.6</v>
+      </c>
+      <c r="E46" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>19</v>
+      </c>
+      <c r="B47" s="2">
+        <v>1119.9000000000001</v>
+      </c>
+      <c r="D47" s="1">
+        <v>25.5</v>
+      </c>
+      <c r="E47" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>20</v>
+      </c>
+      <c r="B48" s="2">
+        <v>1119.9000000000001</v>
+      </c>
+      <c r="D48" s="1">
+        <v>34</v>
+      </c>
+      <c r="E48" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>21</v>
+      </c>
+      <c r="B49" s="2">
+        <v>1127.9000000000001</v>
+      </c>
+      <c r="C49">
+        <v>2</v>
+      </c>
+      <c r="D49" s="1">
+        <v>22.9</v>
+      </c>
+      <c r="E49" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>22</v>
+      </c>
+      <c r="B50" s="2">
+        <v>1127.9000000000001</v>
+      </c>
+      <c r="D50" s="1">
+        <v>28.3</v>
+      </c>
+      <c r="E50" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>23</v>
+      </c>
+      <c r="B51" s="2">
+        <v>1127.9000000000001</v>
+      </c>
+      <c r="D51" s="1">
+        <v>32.700000000000003</v>
+      </c>
+      <c r="E51" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>24</v>
+      </c>
+      <c r="B52" s="2">
+        <v>1140.4000000000001</v>
+      </c>
+      <c r="C52">
+        <v>2</v>
+      </c>
+      <c r="D52" s="1">
+        <v>22</v>
+      </c>
+      <c r="E52" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>25</v>
+      </c>
+      <c r="B53" s="2">
+        <v>1140.4000000000001</v>
+      </c>
+      <c r="D53" s="1">
+        <v>24.1</v>
+      </c>
+      <c r="E53" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>26</v>
+      </c>
+      <c r="B54" s="2">
+        <v>1140.4000000000001</v>
+      </c>
+      <c r="D54" s="1">
+        <v>28.8</v>
+      </c>
+      <c r="E54" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>27</v>
+      </c>
+      <c r="B55" s="2">
+        <v>1148.4000000000001</v>
+      </c>
+      <c r="C55">
+        <v>2</v>
+      </c>
+      <c r="D55" s="1">
+        <v>26.6</v>
+      </c>
+      <c r="E55" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>28</v>
+      </c>
+      <c r="B56" s="2">
+        <v>1148.4000000000001</v>
+      </c>
+      <c r="D56" s="1">
+        <v>28.6</v>
+      </c>
+      <c r="E56" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>29</v>
+      </c>
+      <c r="B57" s="2">
+        <v>1148.4000000000001</v>
+      </c>
+      <c r="D57" s="1">
+        <v>32.4</v>
+      </c>
+      <c r="E57" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>30</v>
+      </c>
+      <c r="B58" s="2">
+        <v>1148.4000000000001</v>
+      </c>
+      <c r="D58" s="1">
+        <v>35.1</v>
+      </c>
+      <c r="E58" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>31</v>
+      </c>
+      <c r="B59" s="2">
+        <v>1182.3</v>
+      </c>
+      <c r="C59">
+        <v>2</v>
+      </c>
+      <c r="D59" s="1">
+        <v>23.9</v>
+      </c>
+      <c r="E59" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>32</v>
+      </c>
+      <c r="B60" s="2">
+        <v>1184.4000000000001</v>
+      </c>
+      <c r="C60">
+        <v>2</v>
+      </c>
+      <c r="D60" s="1">
+        <v>34.5</v>
+      </c>
+      <c r="E60" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>33</v>
+      </c>
+      <c r="B61" s="2">
+        <v>1184.4000000000001</v>
+      </c>
+      <c r="D61" s="1">
+        <v>42.2</v>
+      </c>
+      <c r="E61" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>34</v>
+      </c>
+      <c r="B62" s="2">
+        <v>1184.4000000000001</v>
+      </c>
+      <c r="D62" s="1">
+        <v>48.4</v>
+      </c>
+      <c r="E62" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>35</v>
+      </c>
+      <c r="B63" s="2">
+        <v>1195.4000000000001</v>
+      </c>
+      <c r="C63">
+        <v>2</v>
+      </c>
+      <c r="D63" s="1">
+        <v>34.200000000000003</v>
+      </c>
+      <c r="E63" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>36</v>
+      </c>
+      <c r="B64" s="2">
+        <v>1200.9000000000001</v>
+      </c>
+      <c r="C64">
+        <v>2</v>
+      </c>
+      <c r="D64" s="1">
+        <v>27.4</v>
+      </c>
+      <c r="E64" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>37</v>
+      </c>
+      <c r="B65" s="2">
+        <v>1212.9000000000001</v>
+      </c>
+      <c r="C65">
+        <v>2</v>
+      </c>
+      <c r="D65" s="1">
+        <v>27.9</v>
+      </c>
+      <c r="E65" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>38</v>
+      </c>
+      <c r="B66" s="2">
+        <v>1212.9000000000001</v>
+      </c>
+      <c r="D66" s="1">
+        <v>35.4</v>
+      </c>
+      <c r="E66" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>39</v>
+      </c>
+      <c r="B67" s="2">
+        <v>1221.4000000000001</v>
+      </c>
+      <c r="C67">
+        <v>2</v>
+      </c>
+      <c r="D67" s="1">
+        <v>27.2</v>
+      </c>
+      <c r="E67" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>40</v>
+      </c>
+      <c r="B68" s="2">
+        <v>1221.4000000000001</v>
+      </c>
+      <c r="D68" s="1">
+        <v>30.5</v>
+      </c>
+      <c r="E68" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>41</v>
+      </c>
+      <c r="B69" s="2">
+        <v>1221.4000000000001</v>
+      </c>
+      <c r="D69" s="1">
+        <v>32.9</v>
+      </c>
+      <c r="E69" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>42</v>
+      </c>
+      <c r="B70" s="2">
+        <v>1221.4000000000001</v>
+      </c>
+      <c r="D70" s="1">
+        <v>34.700000000000003</v>
+      </c>
+      <c r="E70" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>43</v>
+      </c>
+      <c r="B71" s="2">
+        <v>1221.4000000000001</v>
+      </c>
+      <c r="D71" s="1">
+        <v>36.9</v>
+      </c>
+      <c r="E71" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>44</v>
+      </c>
+      <c r="B72" s="2">
+        <v>1221.4000000000001</v>
+      </c>
+      <c r="D72" s="1">
+        <v>39.200000000000003</v>
+      </c>
+      <c r="E72" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>45</v>
+      </c>
+      <c r="B73" s="2">
+        <v>1229.5</v>
+      </c>
+      <c r="C73">
+        <v>2</v>
+      </c>
+      <c r="D73" s="1">
+        <v>20.3</v>
+      </c>
+      <c r="E73" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>46</v>
+      </c>
+      <c r="B74" s="2">
+        <v>1229.5</v>
+      </c>
+      <c r="D74" s="1">
+        <v>23.3</v>
+      </c>
+      <c r="E74" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>47</v>
+      </c>
+      <c r="B75" s="2">
+        <v>1235.5</v>
+      </c>
+      <c r="C75">
+        <v>1</v>
+      </c>
+      <c r="D75" s="1">
+        <v>26.2</v>
+      </c>
+      <c r="E75" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>48</v>
+      </c>
+      <c r="B76" s="2">
+        <v>1235.5</v>
+      </c>
+      <c r="D76" s="1">
+        <v>27.9</v>
+      </c>
+      <c r="E76" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>49</v>
+      </c>
+      <c r="B77" s="2">
+        <v>1250</v>
+      </c>
+      <c r="C77">
+        <v>2</v>
+      </c>
+      <c r="D77" s="1">
+        <v>21.5</v>
+      </c>
+      <c r="E77" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>50</v>
+      </c>
+      <c r="B78" s="2">
+        <v>1250</v>
+      </c>
+      <c r="D78" s="1">
+        <v>23.5</v>
+      </c>
+      <c r="E78" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>51</v>
+      </c>
+      <c r="B79" s="2">
+        <v>1286</v>
+      </c>
+      <c r="C79">
+        <v>2</v>
+      </c>
+      <c r="D79" s="1">
+        <v>27.1</v>
+      </c>
+      <c r="E79" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>52</v>
+      </c>
+      <c r="B80" s="2">
+        <v>1286</v>
+      </c>
+      <c r="D80" s="1">
+        <v>32.1</v>
+      </c>
+      <c r="E80" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>53</v>
+      </c>
+      <c r="B81" s="2">
+        <v>1286</v>
+      </c>
+      <c r="D81" s="1">
+        <v>39.1</v>
+      </c>
+      <c r="E81" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>54</v>
+      </c>
+      <c r="B82" s="2">
+        <v>1323</v>
+      </c>
+      <c r="C82">
+        <v>2</v>
+      </c>
+      <c r="D82" s="1">
+        <v>25.6</v>
+      </c>
+      <c r="E82" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>55</v>
+      </c>
+      <c r="B83" s="2">
+        <v>1323</v>
+      </c>
+      <c r="D83" s="1">
+        <v>27.1</v>
+      </c>
+      <c r="E83" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>56</v>
+      </c>
+      <c r="B84" s="2">
+        <v>1323</v>
+      </c>
+      <c r="D84" s="1">
+        <v>28.2</v>
+      </c>
+      <c r="E84" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>57</v>
+      </c>
+      <c r="B85" s="2">
+        <v>1323</v>
+      </c>
+      <c r="D85" s="1">
+        <v>29.8</v>
+      </c>
+      <c r="E85" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>58</v>
+      </c>
+      <c r="B86" s="2">
+        <v>1323</v>
+      </c>
+      <c r="D86" s="1">
+        <v>31.8</v>
+      </c>
+      <c r="E86" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>59</v>
+      </c>
+      <c r="B87" s="2">
+        <v>1331</v>
+      </c>
+      <c r="C87">
+        <v>2</v>
+      </c>
+      <c r="D87" s="1">
+        <v>33.6</v>
+      </c>
+      <c r="E87" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>60</v>
+      </c>
+      <c r="B88" s="2">
+        <v>1366.9</v>
+      </c>
+      <c r="C88">
+        <v>2</v>
+      </c>
+      <c r="D88" s="1">
+        <v>32.9</v>
+      </c>
+      <c r="E88" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>61</v>
+      </c>
+      <c r="B89" s="2">
+        <v>1366.9</v>
+      </c>
+      <c r="D89" s="1">
+        <v>37.799999999999997</v>
+      </c>
+      <c r="E89" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <v>62</v>
+      </c>
+      <c r="B90" s="2">
+        <v>1366.9</v>
+      </c>
+      <c r="D90" s="1">
+        <v>39.1</v>
+      </c>
+      <c r="E90" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <v>63</v>
+      </c>
+      <c r="B91" s="2">
+        <v>1366.9</v>
+      </c>
+      <c r="D91" s="1">
+        <v>42</v>
+      </c>
+      <c r="E91" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <v>64</v>
+      </c>
+      <c r="B92" s="2">
+        <v>1366.9</v>
+      </c>
+      <c r="D92" s="1">
+        <v>45</v>
+      </c>
+      <c r="E92" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <v>65</v>
+      </c>
+      <c r="B93" s="2">
+        <v>1366.9</v>
+      </c>
+      <c r="D93" s="1">
+        <v>46.5</v>
+      </c>
+      <c r="E93" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A94">
+        <v>66</v>
+      </c>
+      <c r="B94" s="2">
+        <v>1366.9</v>
+      </c>
+      <c r="D94" s="1">
+        <v>47.8</v>
+      </c>
+      <c r="E94" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A95">
+        <v>94</v>
+      </c>
+      <c r="B95" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C95" t="s">
+        <v>0</v>
+      </c>
+      <c r="D95" s="1">
+        <v>19.8</v>
+      </c>
+      <c r="E95" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A96">
+        <v>95</v>
+      </c>
+      <c r="B96" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D96" s="1">
+        <v>21.4</v>
+      </c>
+      <c r="E96" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A97">
+        <v>96</v>
+      </c>
+      <c r="B97" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C97" t="s">
+        <v>0</v>
+      </c>
+      <c r="D97" s="1">
+        <v>29.7</v>
+      </c>
+      <c r="E97" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A98">
+        <v>97</v>
+      </c>
+      <c r="B98" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D98" s="1">
+        <v>30.6</v>
+      </c>
+      <c r="E98" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A99">
+        <v>98</v>
+      </c>
+      <c r="B99" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D99" s="1">
+        <v>37.200000000000003</v>
+      </c>
+      <c r="E99" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A100">
+        <v>99</v>
+      </c>
+      <c r="B100" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D100" s="1">
+        <v>45.6</v>
+      </c>
+      <c r="E100" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A101">
+        <v>132</v>
+      </c>
+      <c r="B101" s="2">
+        <v>945.4</v>
+      </c>
+      <c r="D101" s="1">
+        <v>33.5</v>
+      </c>
+      <c r="E101" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A102">
+        <v>133</v>
+      </c>
+      <c r="B102" s="2">
+        <v>957.9</v>
+      </c>
+      <c r="C102">
+        <v>2</v>
+      </c>
+      <c r="D102" s="1">
+        <v>30.3</v>
+      </c>
+      <c r="E102" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A103">
+        <v>134</v>
+      </c>
+      <c r="B103" s="2">
+        <v>965.9</v>
+      </c>
+      <c r="C103">
+        <v>2</v>
+      </c>
+      <c r="D103" s="1">
+        <v>22.6</v>
+      </c>
+      <c r="E103" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A104">
+        <v>135</v>
+      </c>
+      <c r="B104" s="2">
+        <v>965.9</v>
+      </c>
+      <c r="D104" s="1">
+        <v>27.2</v>
+      </c>
+      <c r="E104" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A105">
+        <v>136</v>
+      </c>
+      <c r="B105" s="2">
+        <v>965.9</v>
+      </c>
+      <c r="D105" s="1">
+        <v>31.5</v>
+      </c>
+      <c r="E105" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A106">
+        <v>137</v>
+      </c>
+      <c r="B106" s="2">
+        <v>965.9</v>
+      </c>
+      <c r="D106" s="1">
+        <v>35.700000000000003</v>
+      </c>
+      <c r="E106" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A107">
+        <v>138</v>
+      </c>
+      <c r="B107" s="2">
+        <v>974.4</v>
+      </c>
+      <c r="C107">
+        <v>2</v>
+      </c>
+      <c r="D107" s="1">
+        <v>22</v>
+      </c>
+      <c r="E107" s="1">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A108">
+        <v>139</v>
+      </c>
+      <c r="B108" s="2">
+        <v>974.4</v>
+      </c>
+      <c r="D108" s="1">
+        <v>22.9</v>
+      </c>
+      <c r="E108" s="1">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A109">
+        <v>140</v>
+      </c>
+      <c r="B109" s="2">
+        <v>982.3</v>
+      </c>
+      <c r="C109">
+        <v>2</v>
+      </c>
+      <c r="D109" s="1">
+        <v>16.3</v>
+      </c>
+      <c r="E109" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A110">
+        <v>141</v>
+      </c>
+      <c r="B110" s="2">
+        <v>982.3</v>
+      </c>
+      <c r="D110" s="1">
+        <v>19.399999999999999</v>
+      </c>
+      <c r="E110" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A111">
+        <v>142</v>
+      </c>
+      <c r="B111" s="2">
+        <v>994.9</v>
+      </c>
+      <c r="C111">
+        <v>2</v>
+      </c>
+      <c r="D111" s="1">
+        <v>21</v>
+      </c>
+      <c r="E111" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A112">
+        <v>100</v>
+      </c>
+      <c r="B112" s="2">
+        <v>739.3</v>
+      </c>
+      <c r="C112">
+        <v>2</v>
+      </c>
+      <c r="D112" s="1">
+        <v>13</v>
+      </c>
+      <c r="E112" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A113">
+        <v>101</v>
+      </c>
+      <c r="B113" s="2">
+        <v>759.8</v>
+      </c>
+      <c r="C113">
+        <v>2</v>
+      </c>
+      <c r="D113" s="1">
+        <v>13.5</v>
+      </c>
+      <c r="E113" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A114">
+        <v>102</v>
+      </c>
+      <c r="B114" s="2">
+        <v>779.3</v>
+      </c>
+      <c r="C114">
+        <v>2</v>
+      </c>
+      <c r="D114" s="1">
+        <v>18.600000000000001</v>
+      </c>
+      <c r="E114" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A115">
+        <v>103</v>
+      </c>
+      <c r="B115" s="2">
+        <v>779.3</v>
+      </c>
+      <c r="D115" s="1">
+        <v>19.8</v>
+      </c>
+      <c r="E115" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A116">
+        <v>104</v>
+      </c>
+      <c r="B116" s="2">
+        <v>799.8</v>
+      </c>
+      <c r="C116">
+        <v>2</v>
+      </c>
+      <c r="D116" s="1">
+        <v>22.5</v>
+      </c>
+      <c r="E116" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A117">
+        <v>105</v>
+      </c>
+      <c r="B117" s="2">
+        <v>820.3</v>
+      </c>
+      <c r="C117">
+        <v>2</v>
+      </c>
+      <c r="D117" s="1">
+        <v>13.9</v>
+      </c>
+      <c r="E117" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A118">
+        <v>106</v>
+      </c>
+      <c r="B118" s="2">
+        <v>820.3</v>
+      </c>
+      <c r="D118" s="1">
+        <v>16.2</v>
+      </c>
+      <c r="E118" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A119">
+        <v>107</v>
+      </c>
+      <c r="B119" s="2">
+        <v>820.3</v>
+      </c>
+      <c r="D119" s="1">
+        <v>24.2</v>
+      </c>
+      <c r="E119" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A120">
+        <v>108</v>
+      </c>
+      <c r="B120" s="2">
+        <v>832.8</v>
+      </c>
+      <c r="C120">
+        <v>2</v>
+      </c>
+      <c r="D120" s="1">
+        <v>18.2</v>
+      </c>
+      <c r="E120" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A121">
+        <v>109</v>
+      </c>
+      <c r="B121" s="2">
+        <v>832.8</v>
+      </c>
+      <c r="D121" s="1">
+        <v>23.7</v>
+      </c>
+      <c r="E121" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A122">
+        <v>110</v>
+      </c>
+      <c r="B122" s="2">
+        <v>840.8</v>
+      </c>
+      <c r="C122">
+        <v>2</v>
+      </c>
+      <c r="D122" s="1">
+        <v>14.7</v>
+      </c>
+      <c r="E122" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A123">
+        <v>111</v>
+      </c>
+      <c r="B123" s="2">
+        <v>840.8</v>
+      </c>
+      <c r="D123" s="1">
+        <v>15.4</v>
+      </c>
+      <c r="E123" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A124">
+        <v>112</v>
+      </c>
+      <c r="B124" s="2">
+        <v>860.3</v>
+      </c>
+      <c r="C124">
+        <v>2</v>
+      </c>
+      <c r="D124" s="1">
+        <v>15.3</v>
+      </c>
+      <c r="E124" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A125">
+        <v>113</v>
+      </c>
+      <c r="B125" s="2">
+        <v>860.3</v>
+      </c>
+      <c r="D125" s="1">
+        <v>18.600000000000001</v>
+      </c>
+      <c r="E125" s="1">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A126">
+        <v>114</v>
+      </c>
+      <c r="B126" s="2">
+        <v>860.3</v>
+      </c>
+      <c r="D126" s="1">
+        <v>19.600000000000001</v>
+      </c>
+      <c r="E126" s="1">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A127">
+        <v>115</v>
+      </c>
+      <c r="B127" s="2">
+        <v>860.3</v>
+      </c>
+      <c r="D127" s="1">
+        <v>20.2</v>
+      </c>
+      <c r="E127" s="1">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A128">
+        <v>116</v>
+      </c>
+      <c r="B128" s="2">
+        <v>860.3</v>
+      </c>
+      <c r="D128" s="1">
+        <v>22.3</v>
+      </c>
+      <c r="E128" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A129">
+        <v>117</v>
+      </c>
+      <c r="B129" s="2">
+        <v>864.3</v>
+      </c>
+      <c r="C129">
+        <v>2</v>
+      </c>
+      <c r="D129" s="1">
+        <v>22.8</v>
+      </c>
+      <c r="E129" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A130">
+        <v>118</v>
+      </c>
+      <c r="B130" s="2">
+        <v>867.3</v>
+      </c>
+      <c r="C130">
+        <v>2</v>
+      </c>
+      <c r="D130" s="1">
+        <v>29.7</v>
+      </c>
+      <c r="E130" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A131">
+        <v>119</v>
+      </c>
+      <c r="B131" s="2">
+        <v>893.3</v>
+      </c>
+      <c r="C131">
+        <v>2</v>
+      </c>
+      <c r="D131" s="1">
+        <v>20.7</v>
+      </c>
+      <c r="E131" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A132">
+        <v>120</v>
+      </c>
+      <c r="B132" s="2">
+        <v>893.3</v>
+      </c>
+      <c r="D132" s="1">
+        <v>29.7</v>
+      </c>
+      <c r="E132" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A133">
+        <v>121</v>
+      </c>
+      <c r="B133" s="2">
+        <v>901.4</v>
+      </c>
+      <c r="C133">
+        <v>2</v>
+      </c>
+      <c r="D133" s="1">
+        <v>14.7</v>
+      </c>
+      <c r="E133" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A134">
+        <v>122</v>
+      </c>
+      <c r="B134" s="2">
+        <v>901.4</v>
+      </c>
+      <c r="D134" s="1">
+        <v>17.7</v>
+      </c>
+      <c r="E134" s="1">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A135">
+        <v>123</v>
+      </c>
+      <c r="B135" s="2">
+        <v>901.4</v>
+      </c>
+      <c r="D135" s="1">
+        <v>18.2</v>
+      </c>
+      <c r="E135" s="1">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A136">
+        <v>124</v>
+      </c>
+      <c r="B136" s="2">
+        <v>913.9</v>
+      </c>
+      <c r="C136">
+        <v>2</v>
+      </c>
+      <c r="D136" s="1">
+        <v>18.7</v>
+      </c>
+      <c r="E136" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A137">
+        <v>125</v>
+      </c>
+      <c r="B137" s="2">
+        <v>913.9</v>
+      </c>
+      <c r="D137" s="1">
+        <v>20.100000000000001</v>
+      </c>
+      <c r="E137" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A138">
+        <v>126</v>
+      </c>
+      <c r="B138" s="2">
+        <v>921.9</v>
+      </c>
+      <c r="C138">
+        <v>2</v>
+      </c>
+      <c r="D138" s="1">
+        <v>16.5</v>
+      </c>
+      <c r="E138" s="1">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A139">
+        <v>127</v>
+      </c>
+      <c r="B139" s="2">
+        <v>937.4</v>
+      </c>
+      <c r="C139">
+        <v>2</v>
+      </c>
+      <c r="D139" s="1">
+        <v>27.8</v>
+      </c>
+      <c r="E139" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A140">
+        <v>128</v>
+      </c>
+      <c r="B140" s="2">
+        <v>941.3</v>
+      </c>
+      <c r="C140">
+        <v>2</v>
+      </c>
+      <c r="D140" s="1">
+        <v>15.6</v>
+      </c>
+      <c r="E140" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A141">
+        <v>129</v>
+      </c>
+      <c r="B141" s="2">
+        <v>941.3</v>
+      </c>
+      <c r="D141" s="1">
+        <v>18.899999999999999</v>
+      </c>
+      <c r="E141" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A142">
+        <v>130</v>
+      </c>
+      <c r="B142" s="2">
+        <v>941.3</v>
+      </c>
+      <c r="D142" s="1">
+        <v>20.100000000000001</v>
+      </c>
+      <c r="E142" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A143">
+        <v>131</v>
+      </c>
+      <c r="B143" s="2">
+        <v>945.4</v>
+      </c>
+      <c r="C143">
+        <v>2</v>
+      </c>
+      <c r="D143" s="1">
+        <v>25.6</v>
+      </c>
+      <c r="E143" s="1">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="A2:E143">
+    <sortCondition ref="A2:A143"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Adds controls for EIC smoothing parameters to script and updates example data accordingly
</commit_message>
<xml_diff>
--- a/QuantAnalysis/example_data_EIC_RT.xlsx
+++ b/QuantAnalysis/example_data_EIC_RT.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="45" windowWidth="20115" windowHeight="11310" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="45" windowWidth="20115" windowHeight="11310" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="5" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="6" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="7" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="8" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="14">
   <si>
     <t>1; 2</t>
   </si>
@@ -52,6 +53,12 @@
   </si>
   <si>
     <t>AVG_RTW</t>
+  </si>
+  <si>
+    <t>SmthWidth</t>
+  </si>
+  <si>
+    <t>SmthCycles</t>
   </si>
 </sst>
 </file>
@@ -4364,7 +4371,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E143"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H91" sqref="H91"/>
     </sheetView>
   </sheetViews>
@@ -6557,4 +6564,3060 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G143"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q139" sqref="Q139"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="16.5703125" customWidth="1"/>
+    <col min="3" max="3" width="8.7109375" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" customWidth="1"/>
+    <col min="7" max="7" width="11.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>67</v>
+      </c>
+      <c r="B2" s="2">
+        <v>1367</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+      <c r="D2" s="1">
+        <v>38</v>
+      </c>
+      <c r="E2" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="F2">
+        <v>2.544</v>
+      </c>
+      <c r="G2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>68</v>
+      </c>
+      <c r="B3" s="2">
+        <v>1367</v>
+      </c>
+      <c r="D3" s="1">
+        <v>38.799999999999997</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="F3">
+        <v>3.33</v>
+      </c>
+      <c r="G3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>69</v>
+      </c>
+      <c r="B4" s="2">
+        <v>1367</v>
+      </c>
+      <c r="D4" s="1">
+        <v>41.6</v>
+      </c>
+      <c r="E4" s="1">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>2.544</v>
+      </c>
+      <c r="G4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>70</v>
+      </c>
+      <c r="B5" s="2">
+        <v>1367</v>
+      </c>
+      <c r="D5" s="1">
+        <v>42.6</v>
+      </c>
+      <c r="E5" s="1">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>3.33</v>
+      </c>
+      <c r="G5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>71</v>
+      </c>
+      <c r="B6" s="2">
+        <v>1367</v>
+      </c>
+      <c r="D6" s="1">
+        <v>45</v>
+      </c>
+      <c r="E6" s="1">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>2.544</v>
+      </c>
+      <c r="G6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>72</v>
+      </c>
+      <c r="B7" s="2">
+        <v>1367</v>
+      </c>
+      <c r="D7" s="1">
+        <v>46.5</v>
+      </c>
+      <c r="E7" s="1">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>3.33</v>
+      </c>
+      <c r="G7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>73</v>
+      </c>
+      <c r="B8" s="2">
+        <v>1367</v>
+      </c>
+      <c r="D8" s="1">
+        <v>47.8</v>
+      </c>
+      <c r="E8" s="1">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>2.544</v>
+      </c>
+      <c r="G8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>74</v>
+      </c>
+      <c r="B9" s="2">
+        <v>1367</v>
+      </c>
+      <c r="D9" s="1">
+        <v>48.9</v>
+      </c>
+      <c r="E9" s="1">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>3.33</v>
+      </c>
+      <c r="G9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>75</v>
+      </c>
+      <c r="B10" s="2">
+        <v>1367</v>
+      </c>
+      <c r="D10" s="1">
+        <v>51</v>
+      </c>
+      <c r="E10" s="1">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>2.544</v>
+      </c>
+      <c r="G10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>76</v>
+      </c>
+      <c r="B11" s="2">
+        <v>1404</v>
+      </c>
+      <c r="C11">
+        <v>2</v>
+      </c>
+      <c r="D11" s="1">
+        <v>30.3</v>
+      </c>
+      <c r="E11" s="1">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>3.33</v>
+      </c>
+      <c r="G11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>77</v>
+      </c>
+      <c r="B12" s="2">
+        <v>1404</v>
+      </c>
+      <c r="D12" s="1">
+        <v>33</v>
+      </c>
+      <c r="E12" s="1">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>2.544</v>
+      </c>
+      <c r="G12">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>78</v>
+      </c>
+      <c r="B13" s="2">
+        <v>1404</v>
+      </c>
+      <c r="D13" s="1">
+        <v>37.1</v>
+      </c>
+      <c r="E13" s="1">
+        <v>1</v>
+      </c>
+      <c r="F13">
+        <v>3.33</v>
+      </c>
+      <c r="G13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>79</v>
+      </c>
+      <c r="B14" s="2">
+        <v>1422</v>
+      </c>
+      <c r="C14">
+        <v>2</v>
+      </c>
+      <c r="D14" s="1">
+        <v>37.200000000000003</v>
+      </c>
+      <c r="E14" s="1">
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <v>2.544</v>
+      </c>
+      <c r="G14">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>80</v>
+      </c>
+      <c r="B15" s="2">
+        <v>1468.5</v>
+      </c>
+      <c r="C15">
+        <v>2</v>
+      </c>
+      <c r="D15" s="1">
+        <v>28.7</v>
+      </c>
+      <c r="E15" s="1">
+        <v>1</v>
+      </c>
+      <c r="F15">
+        <v>3.33</v>
+      </c>
+      <c r="G15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>81</v>
+      </c>
+      <c r="B16" s="2">
+        <v>1468.5</v>
+      </c>
+      <c r="D16" s="1">
+        <v>30.6</v>
+      </c>
+      <c r="E16" s="1">
+        <v>1</v>
+      </c>
+      <c r="F16">
+        <v>2.544</v>
+      </c>
+      <c r="G16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>82</v>
+      </c>
+      <c r="B17" s="2">
+        <v>1468.5</v>
+      </c>
+      <c r="D17" s="1">
+        <v>32.200000000000003</v>
+      </c>
+      <c r="E17" s="1">
+        <v>1</v>
+      </c>
+      <c r="F17">
+        <v>3.33</v>
+      </c>
+      <c r="G17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>83</v>
+      </c>
+      <c r="B18" s="2">
+        <v>1468.5</v>
+      </c>
+      <c r="D18" s="1">
+        <v>34.299999999999997</v>
+      </c>
+      <c r="E18" s="1">
+        <v>1</v>
+      </c>
+      <c r="F18">
+        <v>2.544</v>
+      </c>
+      <c r="G18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>84</v>
+      </c>
+      <c r="B19" s="2">
+        <v>1468.5</v>
+      </c>
+      <c r="D19" s="1">
+        <v>41.9</v>
+      </c>
+      <c r="E19" s="1">
+        <v>1</v>
+      </c>
+      <c r="F19">
+        <v>3.33</v>
+      </c>
+      <c r="G19">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>85</v>
+      </c>
+      <c r="B20" s="2">
+        <v>1468.5</v>
+      </c>
+      <c r="D20" s="1">
+        <v>46.6</v>
+      </c>
+      <c r="E20" s="1">
+        <v>1</v>
+      </c>
+      <c r="F20">
+        <v>2.544</v>
+      </c>
+      <c r="G20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>86</v>
+      </c>
+      <c r="B21" s="2">
+        <v>1505.5</v>
+      </c>
+      <c r="C21">
+        <v>2</v>
+      </c>
+      <c r="D21" s="1">
+        <v>23.2</v>
+      </c>
+      <c r="E21" s="1">
+        <v>1</v>
+      </c>
+      <c r="F21">
+        <v>3.33</v>
+      </c>
+      <c r="G21">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>87</v>
+      </c>
+      <c r="B22" s="2">
+        <v>1505.5</v>
+      </c>
+      <c r="D22" s="1">
+        <v>28.1</v>
+      </c>
+      <c r="E22" s="1">
+        <v>1</v>
+      </c>
+      <c r="F22">
+        <v>2.544</v>
+      </c>
+      <c r="G22">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>88</v>
+      </c>
+      <c r="B23" s="2">
+        <v>1505.5</v>
+      </c>
+      <c r="D23" s="1">
+        <v>30.7</v>
+      </c>
+      <c r="E23" s="1">
+        <v>1</v>
+      </c>
+      <c r="F23">
+        <v>3.33</v>
+      </c>
+      <c r="G23">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>89</v>
+      </c>
+      <c r="B24" s="2">
+        <v>1505.5</v>
+      </c>
+      <c r="D24" s="1">
+        <v>32.1</v>
+      </c>
+      <c r="E24" s="1">
+        <v>1</v>
+      </c>
+      <c r="F24">
+        <v>2.544</v>
+      </c>
+      <c r="G24">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>90</v>
+      </c>
+      <c r="B25" s="2">
+        <v>1513.5</v>
+      </c>
+      <c r="C25">
+        <v>2</v>
+      </c>
+      <c r="D25" s="1">
+        <v>35.4</v>
+      </c>
+      <c r="E25" s="1">
+        <v>1</v>
+      </c>
+      <c r="F25">
+        <v>3.33</v>
+      </c>
+      <c r="G25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>91</v>
+      </c>
+      <c r="B26" s="2">
+        <v>1586.5</v>
+      </c>
+      <c r="C26">
+        <v>2</v>
+      </c>
+      <c r="D26" s="1">
+        <v>39.799999999999997</v>
+      </c>
+      <c r="E26" s="1">
+        <v>1</v>
+      </c>
+      <c r="F26">
+        <v>2.544</v>
+      </c>
+      <c r="G26">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>92</v>
+      </c>
+      <c r="B27" s="2">
+        <v>1651</v>
+      </c>
+      <c r="C27">
+        <v>2</v>
+      </c>
+      <c r="D27" s="1">
+        <v>34.1</v>
+      </c>
+      <c r="E27" s="1">
+        <v>1</v>
+      </c>
+      <c r="F27">
+        <v>3.33</v>
+      </c>
+      <c r="G27">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>93</v>
+      </c>
+      <c r="B28" s="2">
+        <v>1651</v>
+      </c>
+      <c r="D28" s="1">
+        <v>44.2</v>
+      </c>
+      <c r="E28" s="1">
+        <v>1</v>
+      </c>
+      <c r="F28">
+        <v>2.544</v>
+      </c>
+      <c r="G28">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>1</v>
+      </c>
+      <c r="B29" s="2">
+        <v>1018.4</v>
+      </c>
+      <c r="C29">
+        <v>2</v>
+      </c>
+      <c r="D29" s="1">
+        <v>30.6</v>
+      </c>
+      <c r="E29" s="1">
+        <v>1</v>
+      </c>
+      <c r="F29">
+        <v>3.33</v>
+      </c>
+      <c r="G29">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>2</v>
+      </c>
+      <c r="B30" s="2">
+        <v>1022.4</v>
+      </c>
+      <c r="C30">
+        <v>2</v>
+      </c>
+      <c r="D30" s="1">
+        <v>20.5</v>
+      </c>
+      <c r="E30" s="1">
+        <v>1</v>
+      </c>
+      <c r="F30">
+        <v>2.544</v>
+      </c>
+      <c r="G30">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>3</v>
+      </c>
+      <c r="B31" s="2">
+        <v>1038.9000000000001</v>
+      </c>
+      <c r="C31">
+        <v>2</v>
+      </c>
+      <c r="D31" s="1">
+        <v>29</v>
+      </c>
+      <c r="E31" s="1">
+        <v>1</v>
+      </c>
+      <c r="F31">
+        <v>3.33</v>
+      </c>
+      <c r="G31">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>4</v>
+      </c>
+      <c r="B32" s="2">
+        <v>1038.9000000000001</v>
+      </c>
+      <c r="D32" s="1">
+        <v>32.1</v>
+      </c>
+      <c r="E32" s="1">
+        <v>1</v>
+      </c>
+      <c r="F32">
+        <v>2.544</v>
+      </c>
+      <c r="G32">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>5</v>
+      </c>
+      <c r="B33" s="2">
+        <v>1038.9000000000001</v>
+      </c>
+      <c r="D33" s="1">
+        <v>35</v>
+      </c>
+      <c r="E33" s="1">
+        <v>1</v>
+      </c>
+      <c r="F33">
+        <v>3.33</v>
+      </c>
+      <c r="G33">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>6</v>
+      </c>
+      <c r="B34" s="2">
+        <v>1038.9000000000001</v>
+      </c>
+      <c r="D34" s="1">
+        <v>36.5</v>
+      </c>
+      <c r="E34" s="1">
+        <v>1</v>
+      </c>
+      <c r="F34">
+        <v>2.544</v>
+      </c>
+      <c r="G34">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>7</v>
+      </c>
+      <c r="B35" s="2">
+        <v>1038.9000000000001</v>
+      </c>
+      <c r="D35" s="1">
+        <v>39.799999999999997</v>
+      </c>
+      <c r="E35" s="1">
+        <v>1</v>
+      </c>
+      <c r="F35">
+        <v>3.33</v>
+      </c>
+      <c r="G35">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>8</v>
+      </c>
+      <c r="B36" s="2">
+        <v>1046.9000000000001</v>
+      </c>
+      <c r="C36">
+        <v>2</v>
+      </c>
+      <c r="D36" s="1">
+        <v>17.5</v>
+      </c>
+      <c r="E36" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="F36">
+        <v>2.544</v>
+      </c>
+      <c r="G36">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>9</v>
+      </c>
+      <c r="B37" s="2">
+        <v>1046.9000000000001</v>
+      </c>
+      <c r="D37" s="1">
+        <v>21.3</v>
+      </c>
+      <c r="E37" s="1">
+        <v>1</v>
+      </c>
+      <c r="F37">
+        <v>3.33</v>
+      </c>
+      <c r="G37">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>10</v>
+      </c>
+      <c r="B38" s="2">
+        <v>1046.9000000000001</v>
+      </c>
+      <c r="D38" s="1">
+        <v>29.9</v>
+      </c>
+      <c r="E38" s="1">
+        <v>1</v>
+      </c>
+      <c r="F38">
+        <v>2.544</v>
+      </c>
+      <c r="G38">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>11</v>
+      </c>
+      <c r="B39" s="2">
+        <v>1059.4000000000001</v>
+      </c>
+      <c r="C39">
+        <v>2</v>
+      </c>
+      <c r="D39" s="1">
+        <v>22.3</v>
+      </c>
+      <c r="E39" s="1">
+        <v>1</v>
+      </c>
+      <c r="F39">
+        <v>3.33</v>
+      </c>
+      <c r="G39">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>12</v>
+      </c>
+      <c r="B40" s="2">
+        <v>1067.4000000000001</v>
+      </c>
+      <c r="C40">
+        <v>2</v>
+      </c>
+      <c r="D40" s="1">
+        <v>19.899999999999999</v>
+      </c>
+      <c r="E40" s="1">
+        <v>1</v>
+      </c>
+      <c r="F40">
+        <v>2.544</v>
+      </c>
+      <c r="G40">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>13</v>
+      </c>
+      <c r="B41" s="2">
+        <v>1067.4000000000001</v>
+      </c>
+      <c r="D41" s="1">
+        <v>25.1</v>
+      </c>
+      <c r="E41" s="1">
+        <v>1</v>
+      </c>
+      <c r="F41">
+        <v>3.33</v>
+      </c>
+      <c r="G41">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>14</v>
+      </c>
+      <c r="B42" s="2">
+        <v>1083.9000000000001</v>
+      </c>
+      <c r="C42">
+        <v>2</v>
+      </c>
+      <c r="D42" s="1">
+        <v>20.399999999999999</v>
+      </c>
+      <c r="E42" s="1">
+        <v>1</v>
+      </c>
+      <c r="F42">
+        <v>2.544</v>
+      </c>
+      <c r="G42">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>15</v>
+      </c>
+      <c r="B43" s="2">
+        <v>1111.4000000000001</v>
+      </c>
+      <c r="C43">
+        <v>2</v>
+      </c>
+      <c r="D43" s="1">
+        <v>29.7</v>
+      </c>
+      <c r="E43" s="1">
+        <v>1</v>
+      </c>
+      <c r="F43">
+        <v>3.33</v>
+      </c>
+      <c r="G43">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>16</v>
+      </c>
+      <c r="B44" s="2">
+        <v>1111.4000000000001</v>
+      </c>
+      <c r="D44" s="1">
+        <v>37.700000000000003</v>
+      </c>
+      <c r="E44" s="1">
+        <v>1</v>
+      </c>
+      <c r="F44">
+        <v>2.544</v>
+      </c>
+      <c r="G44">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>17</v>
+      </c>
+      <c r="B45" s="2">
+        <v>1111.4000000000001</v>
+      </c>
+      <c r="D45" s="1">
+        <v>44.2</v>
+      </c>
+      <c r="E45" s="1">
+        <v>1</v>
+      </c>
+      <c r="F45">
+        <v>3.33</v>
+      </c>
+      <c r="G45">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>18</v>
+      </c>
+      <c r="B46" s="2">
+        <v>1119.9000000000001</v>
+      </c>
+      <c r="C46">
+        <v>2</v>
+      </c>
+      <c r="D46" s="1">
+        <v>21.6</v>
+      </c>
+      <c r="E46" s="1">
+        <v>1</v>
+      </c>
+      <c r="F46">
+        <v>2.544</v>
+      </c>
+      <c r="G46">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>19</v>
+      </c>
+      <c r="B47" s="2">
+        <v>1119.9000000000001</v>
+      </c>
+      <c r="D47" s="1">
+        <v>25.5</v>
+      </c>
+      <c r="E47" s="1">
+        <v>1</v>
+      </c>
+      <c r="F47">
+        <v>3.33</v>
+      </c>
+      <c r="G47">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>20</v>
+      </c>
+      <c r="B48" s="2">
+        <v>1119.9000000000001</v>
+      </c>
+      <c r="D48" s="1">
+        <v>34</v>
+      </c>
+      <c r="E48" s="1">
+        <v>1</v>
+      </c>
+      <c r="F48">
+        <v>2.544</v>
+      </c>
+      <c r="G48">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>21</v>
+      </c>
+      <c r="B49" s="2">
+        <v>1127.9000000000001</v>
+      </c>
+      <c r="C49">
+        <v>2</v>
+      </c>
+      <c r="D49" s="1">
+        <v>22.9</v>
+      </c>
+      <c r="E49" s="1">
+        <v>1</v>
+      </c>
+      <c r="F49">
+        <v>3.33</v>
+      </c>
+      <c r="G49">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>22</v>
+      </c>
+      <c r="B50" s="2">
+        <v>1127.9000000000001</v>
+      </c>
+      <c r="D50" s="1">
+        <v>28.3</v>
+      </c>
+      <c r="E50" s="1">
+        <v>1</v>
+      </c>
+      <c r="F50">
+        <v>2.544</v>
+      </c>
+      <c r="G50">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>23</v>
+      </c>
+      <c r="B51" s="2">
+        <v>1127.9000000000001</v>
+      </c>
+      <c r="D51" s="1">
+        <v>32.700000000000003</v>
+      </c>
+      <c r="E51" s="1">
+        <v>1</v>
+      </c>
+      <c r="F51">
+        <v>3.33</v>
+      </c>
+      <c r="G51">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>24</v>
+      </c>
+      <c r="B52" s="2">
+        <v>1140.4000000000001</v>
+      </c>
+      <c r="C52">
+        <v>2</v>
+      </c>
+      <c r="D52" s="1">
+        <v>22</v>
+      </c>
+      <c r="E52" s="1">
+        <v>1</v>
+      </c>
+      <c r="F52">
+        <v>2.544</v>
+      </c>
+      <c r="G52">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>25</v>
+      </c>
+      <c r="B53" s="2">
+        <v>1140.4000000000001</v>
+      </c>
+      <c r="D53" s="1">
+        <v>24.1</v>
+      </c>
+      <c r="E53" s="1">
+        <v>1</v>
+      </c>
+      <c r="F53">
+        <v>3.33</v>
+      </c>
+      <c r="G53">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>26</v>
+      </c>
+      <c r="B54" s="2">
+        <v>1140.4000000000001</v>
+      </c>
+      <c r="D54" s="1">
+        <v>28.8</v>
+      </c>
+      <c r="E54" s="1">
+        <v>1</v>
+      </c>
+      <c r="F54">
+        <v>2.544</v>
+      </c>
+      <c r="G54">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>27</v>
+      </c>
+      <c r="B55" s="2">
+        <v>1148.4000000000001</v>
+      </c>
+      <c r="C55">
+        <v>2</v>
+      </c>
+      <c r="D55" s="1">
+        <v>26.6</v>
+      </c>
+      <c r="E55" s="1">
+        <v>1</v>
+      </c>
+      <c r="F55">
+        <v>3.33</v>
+      </c>
+      <c r="G55">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>28</v>
+      </c>
+      <c r="B56" s="2">
+        <v>1148.4000000000001</v>
+      </c>
+      <c r="D56" s="1">
+        <v>28.6</v>
+      </c>
+      <c r="E56" s="1">
+        <v>1</v>
+      </c>
+      <c r="F56">
+        <v>2.544</v>
+      </c>
+      <c r="G56">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>29</v>
+      </c>
+      <c r="B57" s="2">
+        <v>1148.4000000000001</v>
+      </c>
+      <c r="D57" s="1">
+        <v>32.4</v>
+      </c>
+      <c r="E57" s="1">
+        <v>1</v>
+      </c>
+      <c r="F57">
+        <v>3.33</v>
+      </c>
+      <c r="G57">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>30</v>
+      </c>
+      <c r="B58" s="2">
+        <v>1148.4000000000001</v>
+      </c>
+      <c r="D58" s="1">
+        <v>35.1</v>
+      </c>
+      <c r="E58" s="1">
+        <v>1</v>
+      </c>
+      <c r="F58">
+        <v>2.544</v>
+      </c>
+      <c r="G58">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>31</v>
+      </c>
+      <c r="B59" s="2">
+        <v>1182.3</v>
+      </c>
+      <c r="C59">
+        <v>2</v>
+      </c>
+      <c r="D59" s="1">
+        <v>23.9</v>
+      </c>
+      <c r="E59" s="1">
+        <v>1</v>
+      </c>
+      <c r="F59">
+        <v>3.33</v>
+      </c>
+      <c r="G59">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>32</v>
+      </c>
+      <c r="B60" s="2">
+        <v>1184.4000000000001</v>
+      </c>
+      <c r="C60">
+        <v>2</v>
+      </c>
+      <c r="D60" s="1">
+        <v>34.5</v>
+      </c>
+      <c r="E60" s="1">
+        <v>1</v>
+      </c>
+      <c r="F60">
+        <v>2.544</v>
+      </c>
+      <c r="G60">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>33</v>
+      </c>
+      <c r="B61" s="2">
+        <v>1184.4000000000001</v>
+      </c>
+      <c r="D61" s="1">
+        <v>42.2</v>
+      </c>
+      <c r="E61" s="1">
+        <v>1</v>
+      </c>
+      <c r="F61">
+        <v>3.33</v>
+      </c>
+      <c r="G61">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>34</v>
+      </c>
+      <c r="B62" s="2">
+        <v>1184.4000000000001</v>
+      </c>
+      <c r="D62" s="1">
+        <v>48.4</v>
+      </c>
+      <c r="E62" s="1">
+        <v>1</v>
+      </c>
+      <c r="F62">
+        <v>2.544</v>
+      </c>
+      <c r="G62">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>35</v>
+      </c>
+      <c r="B63" s="2">
+        <v>1195.4000000000001</v>
+      </c>
+      <c r="C63">
+        <v>2</v>
+      </c>
+      <c r="D63" s="1">
+        <v>34.200000000000003</v>
+      </c>
+      <c r="E63" s="1">
+        <v>1</v>
+      </c>
+      <c r="F63">
+        <v>3.33</v>
+      </c>
+      <c r="G63">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>36</v>
+      </c>
+      <c r="B64" s="2">
+        <v>1200.9000000000001</v>
+      </c>
+      <c r="C64">
+        <v>2</v>
+      </c>
+      <c r="D64" s="1">
+        <v>27.4</v>
+      </c>
+      <c r="E64" s="1">
+        <v>1</v>
+      </c>
+      <c r="F64">
+        <v>2.544</v>
+      </c>
+      <c r="G64">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>37</v>
+      </c>
+      <c r="B65" s="2">
+        <v>1212.9000000000001</v>
+      </c>
+      <c r="C65">
+        <v>2</v>
+      </c>
+      <c r="D65" s="1">
+        <v>27.9</v>
+      </c>
+      <c r="E65" s="1">
+        <v>1</v>
+      </c>
+      <c r="F65">
+        <v>3.33</v>
+      </c>
+      <c r="G65">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>38</v>
+      </c>
+      <c r="B66" s="2">
+        <v>1212.9000000000001</v>
+      </c>
+      <c r="D66" s="1">
+        <v>35.4</v>
+      </c>
+      <c r="E66" s="1">
+        <v>1</v>
+      </c>
+      <c r="F66">
+        <v>2.544</v>
+      </c>
+      <c r="G66">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>39</v>
+      </c>
+      <c r="B67" s="2">
+        <v>1221.4000000000001</v>
+      </c>
+      <c r="C67">
+        <v>2</v>
+      </c>
+      <c r="D67" s="1">
+        <v>27.2</v>
+      </c>
+      <c r="E67" s="1">
+        <v>1</v>
+      </c>
+      <c r="F67">
+        <v>3.33</v>
+      </c>
+      <c r="G67">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>40</v>
+      </c>
+      <c r="B68" s="2">
+        <v>1221.4000000000001</v>
+      </c>
+      <c r="D68" s="1">
+        <v>30.5</v>
+      </c>
+      <c r="E68" s="1">
+        <v>1</v>
+      </c>
+      <c r="F68">
+        <v>2.544</v>
+      </c>
+      <c r="G68">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>41</v>
+      </c>
+      <c r="B69" s="2">
+        <v>1221.4000000000001</v>
+      </c>
+      <c r="D69" s="1">
+        <v>32.9</v>
+      </c>
+      <c r="E69" s="1">
+        <v>1</v>
+      </c>
+      <c r="F69">
+        <v>3.33</v>
+      </c>
+      <c r="G69">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>42</v>
+      </c>
+      <c r="B70" s="2">
+        <v>1221.4000000000001</v>
+      </c>
+      <c r="D70" s="1">
+        <v>34.700000000000003</v>
+      </c>
+      <c r="E70" s="1">
+        <v>1</v>
+      </c>
+      <c r="F70">
+        <v>2.544</v>
+      </c>
+      <c r="G70">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>43</v>
+      </c>
+      <c r="B71" s="2">
+        <v>1221.4000000000001</v>
+      </c>
+      <c r="D71" s="1">
+        <v>36.9</v>
+      </c>
+      <c r="E71" s="1">
+        <v>1</v>
+      </c>
+      <c r="F71">
+        <v>3.33</v>
+      </c>
+      <c r="G71">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>44</v>
+      </c>
+      <c r="B72" s="2">
+        <v>1221.4000000000001</v>
+      </c>
+      <c r="D72" s="1">
+        <v>39.200000000000003</v>
+      </c>
+      <c r="E72" s="1">
+        <v>1</v>
+      </c>
+      <c r="F72">
+        <v>2.544</v>
+      </c>
+      <c r="G72">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>45</v>
+      </c>
+      <c r="B73" s="2">
+        <v>1229.5</v>
+      </c>
+      <c r="C73">
+        <v>2</v>
+      </c>
+      <c r="D73" s="1">
+        <v>20.3</v>
+      </c>
+      <c r="E73" s="1">
+        <v>1</v>
+      </c>
+      <c r="F73">
+        <v>3.33</v>
+      </c>
+      <c r="G73">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>46</v>
+      </c>
+      <c r="B74" s="2">
+        <v>1229.5</v>
+      </c>
+      <c r="D74" s="1">
+        <v>23.3</v>
+      </c>
+      <c r="E74" s="1">
+        <v>1</v>
+      </c>
+      <c r="F74">
+        <v>2.544</v>
+      </c>
+      <c r="G74">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>47</v>
+      </c>
+      <c r="B75" s="2">
+        <v>1235.5</v>
+      </c>
+      <c r="C75">
+        <v>1</v>
+      </c>
+      <c r="D75" s="1">
+        <v>26.2</v>
+      </c>
+      <c r="E75" s="1">
+        <v>1</v>
+      </c>
+      <c r="F75">
+        <v>3.33</v>
+      </c>
+      <c r="G75">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>48</v>
+      </c>
+      <c r="B76" s="2">
+        <v>1235.5</v>
+      </c>
+      <c r="D76" s="1">
+        <v>27.9</v>
+      </c>
+      <c r="E76" s="1">
+        <v>1</v>
+      </c>
+      <c r="F76">
+        <v>2.544</v>
+      </c>
+      <c r="G76">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>49</v>
+      </c>
+      <c r="B77" s="2">
+        <v>1250</v>
+      </c>
+      <c r="C77">
+        <v>2</v>
+      </c>
+      <c r="D77" s="1">
+        <v>21.5</v>
+      </c>
+      <c r="E77" s="1">
+        <v>1</v>
+      </c>
+      <c r="F77">
+        <v>3.33</v>
+      </c>
+      <c r="G77">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>50</v>
+      </c>
+      <c r="B78" s="2">
+        <v>1250</v>
+      </c>
+      <c r="D78" s="1">
+        <v>23.5</v>
+      </c>
+      <c r="E78" s="1">
+        <v>1</v>
+      </c>
+      <c r="F78">
+        <v>2.544</v>
+      </c>
+      <c r="G78">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>51</v>
+      </c>
+      <c r="B79" s="2">
+        <v>1286</v>
+      </c>
+      <c r="C79">
+        <v>2</v>
+      </c>
+      <c r="D79" s="1">
+        <v>27.1</v>
+      </c>
+      <c r="E79" s="1">
+        <v>1</v>
+      </c>
+      <c r="F79">
+        <v>3.33</v>
+      </c>
+      <c r="G79">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>52</v>
+      </c>
+      <c r="B80" s="2">
+        <v>1286</v>
+      </c>
+      <c r="D80" s="1">
+        <v>32.1</v>
+      </c>
+      <c r="E80" s="1">
+        <v>1</v>
+      </c>
+      <c r="F80">
+        <v>2.544</v>
+      </c>
+      <c r="G80">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>53</v>
+      </c>
+      <c r="B81" s="2">
+        <v>1286</v>
+      </c>
+      <c r="D81" s="1">
+        <v>39.1</v>
+      </c>
+      <c r="E81" s="1">
+        <v>1</v>
+      </c>
+      <c r="F81">
+        <v>3.33</v>
+      </c>
+      <c r="G81">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>54</v>
+      </c>
+      <c r="B82" s="2">
+        <v>1323</v>
+      </c>
+      <c r="C82">
+        <v>2</v>
+      </c>
+      <c r="D82" s="1">
+        <v>25.6</v>
+      </c>
+      <c r="E82" s="1">
+        <v>1</v>
+      </c>
+      <c r="F82">
+        <v>2.544</v>
+      </c>
+      <c r="G82">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>55</v>
+      </c>
+      <c r="B83" s="2">
+        <v>1323</v>
+      </c>
+      <c r="D83" s="1">
+        <v>27.1</v>
+      </c>
+      <c r="E83" s="1">
+        <v>1</v>
+      </c>
+      <c r="F83">
+        <v>3.33</v>
+      </c>
+      <c r="G83">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>56</v>
+      </c>
+      <c r="B84" s="2">
+        <v>1323</v>
+      </c>
+      <c r="D84" s="1">
+        <v>28.2</v>
+      </c>
+      <c r="E84" s="1">
+        <v>1</v>
+      </c>
+      <c r="F84">
+        <v>2.544</v>
+      </c>
+      <c r="G84">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>57</v>
+      </c>
+      <c r="B85" s="2">
+        <v>1323</v>
+      </c>
+      <c r="D85" s="1">
+        <v>29.8</v>
+      </c>
+      <c r="E85" s="1">
+        <v>1</v>
+      </c>
+      <c r="F85">
+        <v>3</v>
+      </c>
+      <c r="G85">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>58</v>
+      </c>
+      <c r="B86" s="2">
+        <v>1323</v>
+      </c>
+      <c r="D86" s="1">
+        <v>31.8</v>
+      </c>
+      <c r="E86" s="1">
+        <v>1</v>
+      </c>
+      <c r="F86">
+        <v>2</v>
+      </c>
+      <c r="G86">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>59</v>
+      </c>
+      <c r="B87" s="2">
+        <v>1331</v>
+      </c>
+      <c r="C87">
+        <v>2</v>
+      </c>
+      <c r="D87" s="1">
+        <v>33.6</v>
+      </c>
+      <c r="E87" s="1">
+        <v>1</v>
+      </c>
+      <c r="F87">
+        <v>3</v>
+      </c>
+      <c r="G87">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>60</v>
+      </c>
+      <c r="B88" s="2">
+        <v>1366.9</v>
+      </c>
+      <c r="C88">
+        <v>2</v>
+      </c>
+      <c r="D88" s="1">
+        <v>32.9</v>
+      </c>
+      <c r="E88" s="1">
+        <v>1</v>
+      </c>
+      <c r="F88">
+        <v>3</v>
+      </c>
+      <c r="G88">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>61</v>
+      </c>
+      <c r="B89" s="2">
+        <v>1366.9</v>
+      </c>
+      <c r="D89" s="1">
+        <v>37.799999999999997</v>
+      </c>
+      <c r="E89" s="1">
+        <v>1</v>
+      </c>
+      <c r="F89">
+        <v>2</v>
+      </c>
+      <c r="G89">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <v>62</v>
+      </c>
+      <c r="B90" s="2">
+        <v>1366.9</v>
+      </c>
+      <c r="D90" s="1">
+        <v>39.1</v>
+      </c>
+      <c r="E90" s="1">
+        <v>1</v>
+      </c>
+      <c r="F90">
+        <v>3</v>
+      </c>
+      <c r="G90">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <v>63</v>
+      </c>
+      <c r="B91" s="2">
+        <v>1366.9</v>
+      </c>
+      <c r="D91" s="1">
+        <v>42</v>
+      </c>
+      <c r="E91" s="1">
+        <v>1</v>
+      </c>
+      <c r="F91">
+        <v>2</v>
+      </c>
+      <c r="G91">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <v>64</v>
+      </c>
+      <c r="B92" s="2">
+        <v>1366.9</v>
+      </c>
+      <c r="D92" s="1">
+        <v>45</v>
+      </c>
+      <c r="E92" s="1">
+        <v>1</v>
+      </c>
+      <c r="F92">
+        <v>3</v>
+      </c>
+      <c r="G92">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <v>65</v>
+      </c>
+      <c r="B93" s="2">
+        <v>1366.9</v>
+      </c>
+      <c r="D93" s="1">
+        <v>46.5</v>
+      </c>
+      <c r="E93" s="1">
+        <v>1</v>
+      </c>
+      <c r="F93">
+        <v>3</v>
+      </c>
+      <c r="G93">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A94">
+        <v>66</v>
+      </c>
+      <c r="B94" s="2">
+        <v>1366.9</v>
+      </c>
+      <c r="D94" s="1">
+        <v>47.8</v>
+      </c>
+      <c r="E94" s="1">
+        <v>1</v>
+      </c>
+      <c r="F94">
+        <v>2</v>
+      </c>
+      <c r="G94">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A95">
+        <v>94</v>
+      </c>
+      <c r="B95" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C95" t="s">
+        <v>0</v>
+      </c>
+      <c r="D95" s="1">
+        <v>19.8</v>
+      </c>
+      <c r="E95" s="1">
+        <v>1</v>
+      </c>
+      <c r="F95">
+        <v>3</v>
+      </c>
+      <c r="G95">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A96">
+        <v>95</v>
+      </c>
+      <c r="B96" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D96" s="1">
+        <v>21.4</v>
+      </c>
+      <c r="E96" s="1">
+        <v>1</v>
+      </c>
+      <c r="F96">
+        <v>2</v>
+      </c>
+      <c r="G96">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A97">
+        <v>96</v>
+      </c>
+      <c r="B97" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C97" t="s">
+        <v>0</v>
+      </c>
+      <c r="D97" s="1">
+        <v>29.7</v>
+      </c>
+      <c r="E97" s="1">
+        <v>1</v>
+      </c>
+      <c r="F97">
+        <v>3</v>
+      </c>
+      <c r="G97">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A98">
+        <v>97</v>
+      </c>
+      <c r="B98" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D98" s="1">
+        <v>30.6</v>
+      </c>
+      <c r="E98" s="1">
+        <v>1</v>
+      </c>
+      <c r="F98">
+        <v>3</v>
+      </c>
+      <c r="G98">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A99">
+        <v>98</v>
+      </c>
+      <c r="B99" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D99" s="1">
+        <v>37.200000000000003</v>
+      </c>
+      <c r="E99" s="1">
+        <v>1</v>
+      </c>
+      <c r="F99">
+        <v>2</v>
+      </c>
+      <c r="G99">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A100">
+        <v>99</v>
+      </c>
+      <c r="B100" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D100" s="1">
+        <v>45.6</v>
+      </c>
+      <c r="E100" s="1">
+        <v>1</v>
+      </c>
+      <c r="F100">
+        <v>3</v>
+      </c>
+      <c r="G100">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A101">
+        <v>132</v>
+      </c>
+      <c r="B101" s="2">
+        <v>945.4</v>
+      </c>
+      <c r="D101" s="1">
+        <v>33.5</v>
+      </c>
+      <c r="E101" s="1">
+        <v>1</v>
+      </c>
+      <c r="F101">
+        <v>2</v>
+      </c>
+      <c r="G101">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A102">
+        <v>133</v>
+      </c>
+      <c r="B102" s="2">
+        <v>957.9</v>
+      </c>
+      <c r="C102">
+        <v>2</v>
+      </c>
+      <c r="D102" s="1">
+        <v>30.3</v>
+      </c>
+      <c r="E102" s="1">
+        <v>1</v>
+      </c>
+      <c r="F102">
+        <v>3</v>
+      </c>
+      <c r="G102">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A103">
+        <v>134</v>
+      </c>
+      <c r="B103" s="2">
+        <v>965.9</v>
+      </c>
+      <c r="C103">
+        <v>2</v>
+      </c>
+      <c r="D103" s="1">
+        <v>22.6</v>
+      </c>
+      <c r="E103" s="1">
+        <v>1</v>
+      </c>
+      <c r="F103">
+        <v>3</v>
+      </c>
+      <c r="G103">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A104">
+        <v>135</v>
+      </c>
+      <c r="B104" s="2">
+        <v>965.9</v>
+      </c>
+      <c r="D104" s="1">
+        <v>27.2</v>
+      </c>
+      <c r="E104" s="1">
+        <v>1</v>
+      </c>
+      <c r="F104">
+        <v>2</v>
+      </c>
+      <c r="G104">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A105">
+        <v>136</v>
+      </c>
+      <c r="B105" s="2">
+        <v>965.9</v>
+      </c>
+      <c r="D105" s="1">
+        <v>31.5</v>
+      </c>
+      <c r="E105" s="1">
+        <v>1</v>
+      </c>
+      <c r="F105">
+        <v>3</v>
+      </c>
+      <c r="G105">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A106">
+        <v>137</v>
+      </c>
+      <c r="B106" s="2">
+        <v>965.9</v>
+      </c>
+      <c r="D106" s="1">
+        <v>35.700000000000003</v>
+      </c>
+      <c r="E106" s="1">
+        <v>1</v>
+      </c>
+      <c r="F106">
+        <v>2</v>
+      </c>
+      <c r="G106">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A107">
+        <v>138</v>
+      </c>
+      <c r="B107" s="2">
+        <v>974.4</v>
+      </c>
+      <c r="C107">
+        <v>2</v>
+      </c>
+      <c r="D107" s="1">
+        <v>22</v>
+      </c>
+      <c r="E107" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="F107">
+        <v>3</v>
+      </c>
+      <c r="G107">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A108">
+        <v>139</v>
+      </c>
+      <c r="B108" s="2">
+        <v>974.4</v>
+      </c>
+      <c r="D108" s="1">
+        <v>22.9</v>
+      </c>
+      <c r="E108" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="F108">
+        <v>3</v>
+      </c>
+      <c r="G108">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A109">
+        <v>140</v>
+      </c>
+      <c r="B109" s="2">
+        <v>982.3</v>
+      </c>
+      <c r="C109">
+        <v>2</v>
+      </c>
+      <c r="D109" s="1">
+        <v>16.3</v>
+      </c>
+      <c r="E109" s="1">
+        <v>1</v>
+      </c>
+      <c r="F109">
+        <v>2</v>
+      </c>
+      <c r="G109">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A110">
+        <v>141</v>
+      </c>
+      <c r="B110" s="2">
+        <v>982.3</v>
+      </c>
+      <c r="D110" s="1">
+        <v>19.399999999999999</v>
+      </c>
+      <c r="E110" s="1">
+        <v>1</v>
+      </c>
+      <c r="F110">
+        <v>3</v>
+      </c>
+      <c r="G110">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A111">
+        <v>142</v>
+      </c>
+      <c r="B111" s="2">
+        <v>994.9</v>
+      </c>
+      <c r="C111">
+        <v>2</v>
+      </c>
+      <c r="D111" s="1">
+        <v>21</v>
+      </c>
+      <c r="E111" s="1">
+        <v>1</v>
+      </c>
+      <c r="F111">
+        <v>2</v>
+      </c>
+      <c r="G111">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A112">
+        <v>100</v>
+      </c>
+      <c r="B112" s="2">
+        <v>739.3</v>
+      </c>
+      <c r="C112">
+        <v>2</v>
+      </c>
+      <c r="D112" s="1">
+        <v>13</v>
+      </c>
+      <c r="E112" s="1">
+        <v>1</v>
+      </c>
+      <c r="F112">
+        <v>3</v>
+      </c>
+      <c r="G112">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A113">
+        <v>101</v>
+      </c>
+      <c r="B113" s="2">
+        <v>759.8</v>
+      </c>
+      <c r="C113">
+        <v>2</v>
+      </c>
+      <c r="D113" s="1">
+        <v>13.5</v>
+      </c>
+      <c r="E113" s="1">
+        <v>1</v>
+      </c>
+      <c r="F113">
+        <v>3</v>
+      </c>
+      <c r="G113">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A114">
+        <v>102</v>
+      </c>
+      <c r="B114" s="2">
+        <v>779.3</v>
+      </c>
+      <c r="C114">
+        <v>2</v>
+      </c>
+      <c r="D114" s="1">
+        <v>18.600000000000001</v>
+      </c>
+      <c r="E114" s="1">
+        <v>1</v>
+      </c>
+      <c r="F114">
+        <v>2</v>
+      </c>
+      <c r="G114">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A115">
+        <v>103</v>
+      </c>
+      <c r="B115" s="2">
+        <v>779.3</v>
+      </c>
+      <c r="D115" s="1">
+        <v>19.8</v>
+      </c>
+      <c r="E115" s="1">
+        <v>1</v>
+      </c>
+      <c r="F115">
+        <v>3</v>
+      </c>
+      <c r="G115">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A116">
+        <v>104</v>
+      </c>
+      <c r="B116" s="2">
+        <v>799.8</v>
+      </c>
+      <c r="C116">
+        <v>2</v>
+      </c>
+      <c r="D116" s="1">
+        <v>22.5</v>
+      </c>
+      <c r="E116" s="1">
+        <v>1</v>
+      </c>
+      <c r="F116">
+        <v>2</v>
+      </c>
+      <c r="G116">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A117">
+        <v>105</v>
+      </c>
+      <c r="B117" s="2">
+        <v>820.3</v>
+      </c>
+      <c r="C117">
+        <v>2</v>
+      </c>
+      <c r="D117" s="1">
+        <v>13.9</v>
+      </c>
+      <c r="E117" s="1">
+        <v>1</v>
+      </c>
+      <c r="F117">
+        <v>3</v>
+      </c>
+      <c r="G117">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A118">
+        <v>106</v>
+      </c>
+      <c r="B118" s="2">
+        <v>820.3</v>
+      </c>
+      <c r="D118" s="1">
+        <v>16.2</v>
+      </c>
+      <c r="E118" s="1">
+        <v>1</v>
+      </c>
+      <c r="F118">
+        <v>3</v>
+      </c>
+      <c r="G118">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A119">
+        <v>107</v>
+      </c>
+      <c r="B119" s="2">
+        <v>820.3</v>
+      </c>
+      <c r="D119" s="1">
+        <v>24.2</v>
+      </c>
+      <c r="E119" s="1">
+        <v>1</v>
+      </c>
+      <c r="F119">
+        <v>2</v>
+      </c>
+      <c r="G119">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A120">
+        <v>108</v>
+      </c>
+      <c r="B120" s="2">
+        <v>832.8</v>
+      </c>
+      <c r="C120">
+        <v>2</v>
+      </c>
+      <c r="D120" s="1">
+        <v>18.2</v>
+      </c>
+      <c r="E120" s="1">
+        <v>1</v>
+      </c>
+      <c r="F120">
+        <v>3</v>
+      </c>
+      <c r="G120">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A121">
+        <v>109</v>
+      </c>
+      <c r="B121" s="2">
+        <v>832.8</v>
+      </c>
+      <c r="D121" s="1">
+        <v>23.7</v>
+      </c>
+      <c r="E121" s="1">
+        <v>1</v>
+      </c>
+      <c r="F121">
+        <v>2</v>
+      </c>
+      <c r="G121">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A122">
+        <v>110</v>
+      </c>
+      <c r="B122" s="2">
+        <v>840.8</v>
+      </c>
+      <c r="C122">
+        <v>2</v>
+      </c>
+      <c r="D122" s="1">
+        <v>14.7</v>
+      </c>
+      <c r="E122" s="1">
+        <v>1</v>
+      </c>
+      <c r="F122">
+        <v>3</v>
+      </c>
+      <c r="G122">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A123">
+        <v>111</v>
+      </c>
+      <c r="B123" s="2">
+        <v>840.8</v>
+      </c>
+      <c r="D123" s="1">
+        <v>15.4</v>
+      </c>
+      <c r="E123" s="1">
+        <v>1</v>
+      </c>
+      <c r="F123">
+        <v>3</v>
+      </c>
+      <c r="G123">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A124">
+        <v>112</v>
+      </c>
+      <c r="B124" s="2">
+        <v>860.3</v>
+      </c>
+      <c r="C124">
+        <v>2</v>
+      </c>
+      <c r="D124" s="1">
+        <v>15.3</v>
+      </c>
+      <c r="E124" s="1">
+        <v>1</v>
+      </c>
+      <c r="F124">
+        <v>2</v>
+      </c>
+      <c r="G124">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A125">
+        <v>113</v>
+      </c>
+      <c r="B125" s="2">
+        <v>860.3</v>
+      </c>
+      <c r="D125" s="1">
+        <v>18.600000000000001</v>
+      </c>
+      <c r="E125" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="F125">
+        <v>3</v>
+      </c>
+      <c r="G125">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A126">
+        <v>114</v>
+      </c>
+      <c r="B126" s="2">
+        <v>860.3</v>
+      </c>
+      <c r="D126" s="1">
+        <v>19.600000000000001</v>
+      </c>
+      <c r="E126" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="F126">
+        <v>2</v>
+      </c>
+      <c r="G126">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A127">
+        <v>115</v>
+      </c>
+      <c r="B127" s="2">
+        <v>860.3</v>
+      </c>
+      <c r="D127" s="1">
+        <v>20.2</v>
+      </c>
+      <c r="E127" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="F127">
+        <v>3</v>
+      </c>
+      <c r="G127">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A128">
+        <v>116</v>
+      </c>
+      <c r="B128" s="2">
+        <v>860.3</v>
+      </c>
+      <c r="D128" s="1">
+        <v>22.3</v>
+      </c>
+      <c r="E128" s="1">
+        <v>1</v>
+      </c>
+      <c r="F128">
+        <v>3</v>
+      </c>
+      <c r="G128">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A129">
+        <v>117</v>
+      </c>
+      <c r="B129" s="2">
+        <v>864.3</v>
+      </c>
+      <c r="C129">
+        <v>2</v>
+      </c>
+      <c r="D129" s="1">
+        <v>22.8</v>
+      </c>
+      <c r="E129" s="1">
+        <v>1</v>
+      </c>
+      <c r="F129">
+        <v>2</v>
+      </c>
+      <c r="G129">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A130">
+        <v>118</v>
+      </c>
+      <c r="B130" s="2">
+        <v>867.3</v>
+      </c>
+      <c r="C130">
+        <v>2</v>
+      </c>
+      <c r="D130" s="1">
+        <v>29.7</v>
+      </c>
+      <c r="E130" s="1">
+        <v>1</v>
+      </c>
+      <c r="F130">
+        <v>3</v>
+      </c>
+      <c r="G130">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A131">
+        <v>119</v>
+      </c>
+      <c r="B131" s="2">
+        <v>893.3</v>
+      </c>
+      <c r="C131">
+        <v>2</v>
+      </c>
+      <c r="D131" s="1">
+        <v>20.7</v>
+      </c>
+      <c r="E131" s="1">
+        <v>1</v>
+      </c>
+      <c r="F131">
+        <v>2</v>
+      </c>
+      <c r="G131">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A132">
+        <v>120</v>
+      </c>
+      <c r="B132" s="2">
+        <v>893.3</v>
+      </c>
+      <c r="D132" s="1">
+        <v>29.7</v>
+      </c>
+      <c r="E132" s="1">
+        <v>1</v>
+      </c>
+      <c r="F132">
+        <v>3</v>
+      </c>
+      <c r="G132">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A133">
+        <v>121</v>
+      </c>
+      <c r="B133" s="2">
+        <v>901.4</v>
+      </c>
+      <c r="C133">
+        <v>2</v>
+      </c>
+      <c r="D133" s="1">
+        <v>14.7</v>
+      </c>
+      <c r="E133" s="1">
+        <v>1</v>
+      </c>
+      <c r="F133">
+        <v>3</v>
+      </c>
+      <c r="G133">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A134">
+        <v>122</v>
+      </c>
+      <c r="B134" s="2">
+        <v>901.4</v>
+      </c>
+      <c r="D134" s="1">
+        <v>17.7</v>
+      </c>
+      <c r="E134" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="F134">
+        <v>2</v>
+      </c>
+      <c r="G134">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A135">
+        <v>123</v>
+      </c>
+      <c r="B135" s="2">
+        <v>901.4</v>
+      </c>
+      <c r="D135" s="1">
+        <v>18.2</v>
+      </c>
+      <c r="E135" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="F135">
+        <v>3</v>
+      </c>
+      <c r="G135">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A136">
+        <v>124</v>
+      </c>
+      <c r="B136" s="2">
+        <v>913.9</v>
+      </c>
+      <c r="C136">
+        <v>2</v>
+      </c>
+      <c r="D136" s="1">
+        <v>18.7</v>
+      </c>
+      <c r="E136" s="1">
+        <v>1</v>
+      </c>
+      <c r="F136">
+        <v>2</v>
+      </c>
+      <c r="G136">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A137">
+        <v>125</v>
+      </c>
+      <c r="B137" s="2">
+        <v>913.9</v>
+      </c>
+      <c r="D137" s="1">
+        <v>20.100000000000001</v>
+      </c>
+      <c r="E137" s="1">
+        <v>1</v>
+      </c>
+      <c r="F137">
+        <v>3</v>
+      </c>
+      <c r="G137">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A138">
+        <v>126</v>
+      </c>
+      <c r="B138" s="2">
+        <v>921.9</v>
+      </c>
+      <c r="C138">
+        <v>2</v>
+      </c>
+      <c r="D138" s="1">
+        <v>16.5</v>
+      </c>
+      <c r="E138" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="F138">
+        <v>3</v>
+      </c>
+      <c r="G138">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A139">
+        <v>127</v>
+      </c>
+      <c r="B139" s="2">
+        <v>937.4</v>
+      </c>
+      <c r="C139">
+        <v>2</v>
+      </c>
+      <c r="D139" s="1">
+        <v>27.8</v>
+      </c>
+      <c r="E139" s="1">
+        <v>1</v>
+      </c>
+      <c r="F139">
+        <v>2</v>
+      </c>
+      <c r="G139">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A140">
+        <v>128</v>
+      </c>
+      <c r="B140" s="2">
+        <v>941.3</v>
+      </c>
+      <c r="C140">
+        <v>2</v>
+      </c>
+      <c r="D140" s="1">
+        <v>15.6</v>
+      </c>
+      <c r="E140" s="1">
+        <v>1</v>
+      </c>
+      <c r="F140">
+        <v>3</v>
+      </c>
+      <c r="G140">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A141">
+        <v>129</v>
+      </c>
+      <c r="B141" s="2">
+        <v>941.3</v>
+      </c>
+      <c r="D141" s="1">
+        <v>18.899999999999999</v>
+      </c>
+      <c r="E141" s="1">
+        <v>1</v>
+      </c>
+      <c r="F141">
+        <v>2</v>
+      </c>
+      <c r="G141">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A142">
+        <v>130</v>
+      </c>
+      <c r="B142" s="2">
+        <v>941.3</v>
+      </c>
+      <c r="D142" s="1">
+        <v>20.100000000000001</v>
+      </c>
+      <c r="E142" s="1">
+        <v>1</v>
+      </c>
+      <c r="F142">
+        <v>3</v>
+      </c>
+      <c r="G142">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A143">
+        <v>131</v>
+      </c>
+      <c r="B143" s="2">
+        <v>945.4</v>
+      </c>
+      <c r="C143">
+        <v>2</v>
+      </c>
+      <c r="D143" s="1">
+        <v>25.6</v>
+      </c>
+      <c r="E143" s="1">
+        <v>1</v>
+      </c>
+      <c r="F143">
+        <v>3</v>
+      </c>
+      <c r="G143">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>